<commit_message>
update script, adding new cols
</commit_message>
<xml_diff>
--- a/avito_cars.xlsx
+++ b/avito_cars.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD16"/>
+  <dimension ref="A1:AF22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -579,51 +579,66 @@
           <t>Описание</t>
         </is>
       </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>Владельцев по ПТС</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>Пробег</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>Комплектация</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Москвич 3, 2023</t>
+          <t>Skoda Yeti, 2013</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Москвич</t>
+          <t>Skoda</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>Yeti</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>сегодня в 16:21</t>
+          <t>сегодня в 17:23</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>от 1 692 000</t>
+          <t>739 000</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Пермский край, Пермь, Подлесная ул., 47А</t>
+          <t>Санкт-Петербург, Пушкинский р-н, пос. Шушары, Пулковское ш., 70</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>https://www.avito.ru/perm/avtomobili/moskvich_3_2023_3015860903</t>
+          <t>https://www.avito.ru/sankt-peterburg/avtomobili/skoda_yeti_2013_3122641180</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>2013</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>I (2022—2023)</t>
+          <t>I (2009—2014)</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -633,12 +648,12 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>1.5 MT (150 л.с.)</t>
+          <t>1.2 TSI DSG (105 л.с.)</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>1.5 л</t>
+          <t>1.2 л</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
@@ -648,7 +663,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>Механика</t>
+          <t>Робот</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -663,7 +678,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Чёрный</t>
+          <t>Пурпурный</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
@@ -673,94 +688,114 @@
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>50 л</t>
+          <t>55 л</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>6,4 л/100 км</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>12 с</t>
         </is>
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>4410 мм</t>
+          <t>4223 мм</t>
         </is>
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>1660 мм</t>
+          <t>1691 мм</t>
         </is>
       </c>
       <c r="X2" t="inlineStr">
         <is>
-          <t>150 мм</t>
+          <t>180 мм</t>
         </is>
       </c>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>1510 мм</t>
+          <t>1541 мм</t>
         </is>
       </c>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>1500 мм</t>
+          <t>1537 мм</t>
         </is>
       </c>
       <c r="AA2" t="inlineStr">
         <is>
-          <t>XTC2*************</t>
+          <t>TMBJ*************</t>
         </is>
       </c>
       <c r="AC2" t="inlineStr">
         <is>
-          <t>⚡Новый Москвич за наличные или в кредитОграниченное количество автомобилей в ПермиЗаберите свой Москвич прямо сегодня------------------------Компания САТУРН-Р-АВТО представляет только актуальный склад автомобилей в наличии.✅Мы указываем только реальные условия покупки✅Мы заберем Ваш старый автомобиль и сделаем скидку на новый по программе трейд-ин.✅В наличии всегда большой выбор комплектаций и расцветок автомобилей Москвич ✅Выгодные кредитные программы со сниженной ставкой от 17 банков.✅Доступные программы автострахования КАСКО и ОСАГО от 26 страховых компаний.✅Гарантия на автомобиль 3 ГОДА или 100 000 км пробега в зависимости от того, что наступит ранее.☎️Звоните прямо сейчас и бронируйте ваш Москвич в САТУРН-Р-АВТО------------------------САТУРН-Р-АВТО - официальный дилер Москвич в Перми Пермь, Подлесная, 47А* Цена автомобиля может быть увеличена на сумму установленного дополнительного оборудования. Кредитор ПАО «Росбанк», лицензия ЦБ РФ № 2272 от 28.01.2015 г. Предложение распространяется на новые автомобили Москвич 3.Представленное изображение носит информационный характер, может отличаться от реального товара. Не оферта. Предложение ограничено, подробности уточняйте у менеджеров отдела продаж.</t>
+          <t>• Быстрый выкуп вашего автомобиля: - Выкупаем по рыночной стоимости; - Выкуп в день обращения; - Возможен выкуп кредитного автомобиля; - Специальные условия по программе «Trade-in», обменяем ваш старый авто на новый за 1 час. • Комиссионная продажа вашего автомобиля по вашей цене на условиях бесплатной стоянки. • Рефинансируем ваш автокредит под минимальную процентную ставку. _______________________________________________ Автомобиль представлен официальным дилером Чери Центр Пулково. Покупка в Чери Центр Пулково - это всегда проверенный автомобиль и целый ряд преимуществ: Мы предоставляем бесплатное такси от ст. м. Московский проспект до нашего автоцентра! • ГАРАНТИЯ ЮРИДИЧЕСКОЙ ЧИСТОТЫ: Мы осуществили все необходимые проверки и даём гарантию юридической чистоты всех наших автомобилей. • СТРАХОВАНИЕ КАСКО, ОСАГО: В нашем автоцентре Вы всегда можете осуществить любой вид автострахования. • ТЕХНИЧЕСКАЯ ДИАГНОСТИКА: Мы проверили состояние всех наших автомобилей по 56 пунктам, и предоставляем год гарантии на основные технические узлы. (Со всеми результатами диагностики Вы можете подробнее ознакомиться по телефону либо запросить документы непосредственно в автосалоне) Мы расскажем вам всю правду о состоянии автомобиля. • ПРЕДПРОДАЖНАЯ ПОДГОТОВКА: Мы произвели глубокую химчистку салона и полировку всех кузовных элементов, подготовили автомобиль для дальнейшей эксплуатации. • СПЕЦИАЛЬНЫЕ УСЛОВИЯ ПРИ ПОКУПКЕ АВТОМОБИЛЯ В КРЕДИТ: Предоставляется дополнительная скидка до 150 000 рублей.* • "TRADE-IN" Вашего авто - на представленный в нашей компании. При обмене Вашего автомобиля, также предоставляет дополнительные скидки до 150 000 рублей*. • ОГРОМНЫЙ ВЫБОР ДОПОЛНИТЕЛЬНОГО ОБОРУДОВАНИЯ: У нас вы сможете приобрести дополнительное оборудование на ваш автомобиль (защитные плёнки и покрытия, шины и диски, парктроник, сигнализацию и др. аксессуары). • ТЕСТ-ДРАЙВ: Мы всегда стремимся подобрать для Вас идеальный вариант, поэтому у нас возможно осуществить пробную поездку на любом понравившемся Вам автомобиле. ______________________________________________ • ПРЕИМУЩЕСТВА АВТОКРЕДИТОВАНИЯ: ✓ Автокредит без страховых нагрузок; ✓ По двум документам (паспорт РФ, водительское удостоверение); ✓ Первоначальный взнос от 0%; ✓ Ставка по автокредиту от 7,9%; ✓ Более 15 банков партнеров; ✓ Более 52 различных программ; ✓ Автокредит до 3 000 000 рублей; ✓ Возможность досрочного погашения без комиссий и штрафов. Подача заявки также доступна онлайн: просто позвоните, и кредитный специалист проконсультирует Вас! Если наш автомобиль вас не заинтересовал, то мы поможем вам приобрести любой другой автомобиль в кредит через наш автосалон. Ждём Вас ежедневно с 9 до 21 по адресу: г. Санкт-Петербург, Пулковское шоссе, д. 70 Местонахождение нашего автоцентра на карте вы можете увидеть на последнем фото.  *Данные скидки применяются в зависимости от условий покупки, а также от цены автомобиля.</t>
         </is>
       </c>
       <c r="AD2" t="inlineStr">
         <is>
-          <t>Стандарт</t>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t>93503 км</t>
+        </is>
+      </c>
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t>Active, Ambition, Elegance, Базовая, Experience, Sochi</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ВАЗ (LADA) Niva Legend, 2023</t>
+          <t>Kia Seltos, 2020</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ВАЗ</t>
+          <t>Kia</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>(LADA)</t>
+          <t>Seltos</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>сегодня в 16:01</t>
+          <t>сегодня в 15:52</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>от 815 200</t>
+          <t>2 159 900</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Пермский край, Пермь, Бродовский тракт, 15</t>
+          <t>Санкт-Петербург, Малая Балканская ул., 57</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://www.avito.ru/perm/avtomobili/vaz_lada_niva_legend_2023_3154097427</t>
+          <t>https://www.avito.ru/sankt-peterburg/avtomobili/kia_seltos_2020_3249851748</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>2020</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>I (2021—2023)</t>
+          <t>I (2019—2023)</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -770,12 +805,12 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>1.7 MT (83 л.с.)</t>
+          <t>1.6 AT (123 л.с.)</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>1.7 л</t>
+          <t>1.6 л</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
@@ -785,22 +820,22 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>Механика</t>
+          <t>Автомат</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Полный</t>
+          <t>Передний</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Внедорожник 3-дверный</t>
+          <t>Внедорожник 5-дверный</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Зелёный</t>
+          <t>Красный</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
@@ -810,104 +845,114 @@
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>42 л</t>
+          <t>50 л</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>9,9 л/100 км</t>
+          <t>7,4 л/100 км</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>17 с</t>
+          <t>12,3 с</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>3740 мм</t>
+          <t>4370 мм</t>
         </is>
       </c>
       <c r="W3" t="inlineStr">
         <is>
-          <t>1640 мм</t>
+          <t>1615 мм</t>
         </is>
       </c>
       <c r="X3" t="inlineStr">
         <is>
-          <t>205 мм</t>
+          <t>190 мм</t>
         </is>
       </c>
       <c r="Y3" t="inlineStr">
         <is>
-          <t>1440 мм</t>
+          <t>1575 мм</t>
         </is>
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>1420 мм</t>
+          <t>1584 мм</t>
         </is>
       </c>
       <c r="AA3" t="inlineStr">
         <is>
-          <t>XTA2*************</t>
+          <t>XWEE*************</t>
         </is>
       </c>
       <c r="AC3" t="inlineStr">
         <is>
-          <t>Место осмотраОсмотреть автомобиль можно по адресу: Пермь, Бродовский тракт, 15ДАВ-АВТО — крупная автомобильная компания, услугами которой воспользовались тысячи клиентов. Компания ДАВ-АВТО успешно развивается на рынке автомобильного бизнеса Пермского края уже более 25 лет.В ДАВ-АВТО у Вас есть возможность получить в подарок любые опции на 30000 рублей при покупке новой LADA 🎁. Не упустите возможность выгодно приобрести автомобиль❗️Мы можем предоставить Вам фото или видео презентацию интересующего автомобиля и отправить на почту или в любой удобный мессенджер (Viber, WhatsApp, Telegram).Мы также всегда готовы предложить для Вас:✅ Увлекательная пробная поездка на любой модели LADA в черте города и по бездорожью в удобное для Вас время;✅ Большой склад автомобилей с ЭПТС в наличии;✅ Работает программа утилизации!;✅ Обмен любого автомобиля на новую LADA (принимаем автомобили на обмен в любом состоянии, с ограничениями /штрафами);✅ Рефинансирование Вашего автокредита (мы закроем Ваш действующий автокредит, выкупим автомобиль с учётом остаточной стоимости, рассчитаем сумму доплаты на покупку нового автомобиля);✅ Кредитование и страхование не выходя из автосалона;Сотрудничаем с более 20-ти банками и страховыми компаниями, подбираем оптимальные условия по сроку, ставке и ежемесячному платежу. Рассмотрение заявки в течение 30 минут, одобрение в 99% случаев по одному документу, без справок.✅ Постановка автомобиля на учёт без выезда в ГИБДД, выдача автомобиля с государственными регистрационными знаками;✅ Бесплатное такси до автоцентра (в пределах города).Окончательную стоимость и условия действующих программ интересующего автомобиля уточняйте у менеджеров отдела продаж по телефону указанном в объявлении.Мы стараемся сделать максимально комфортным Ваше пребывание в нашем автоцентре!</t>
+          <t>#cmecMzctMDAyTUw1MC0wMDI2Wk8w Экстерьер Передние и задние брызговики Серебристые накладки на передний и задний бампер Боковые зеркала, окрашенные в цвет кузова Колёсные диски 16-дюймовые с шинами 205/60 R16 Колёсные диски легкосплавные Галогенные фары проекционного типа Противотуманные фары галогенные Двухцветная окраска кузова (опционально) Рейлинги на крыше Запасное колесо малоразмерное Запасное колесо со стальным диском Интерьер Подсветка багажника Регулировка рулевой колонки по высоте Регулировка рулевой колонки по вылету Крючки для крепления сетки в багажнике Задние сиденья со спинками, складывающимися в соотношении 60/40 Вставки серого цвета Отделка руля кожей Отделка рычага КПП кожей Обивка сидений тканевая Полка багажного отделения Приборная панель с 3,5-дюймовым дисплеем Безопасность Устройство вызова экстренных оперативных служб «Эра-Глонасс» Автоматическое запирание дверей при движении Иммобилайзер Центральный замок Крепления детских сидений ISOFIX Система контроля давления в шинах (TPMS) Система помощи при трогании на подъёме (HAC) Система помощи при торможении на склоне (DBC) Система курсовой устойчивости (ESC) Антиблокировочная система (ABS) Передние и задние дисковые тормоза Фронтальная подушка безопасности водителя Фронтальная подушка безопасности переднего пассажира Боковые подушки безопасности Боковые шторки безопасности Система выбора режима движения Drive Mode Select (кроме версий с механической трансмиссией) Датчики парковки задние Камера заднего вида с динамическими линиями парковки Комфорт Мультимедийная система (FM/AM, MP3, RDS) USB-разъём на передней панели 6 динамиков Сиденье водителя с регулировкой по высоте Мультифункциональное рулевое колесо Электростеклоподъёмники передние Электростеклоподъёмники задние Задние сиденья с регулировкой угла наклона Подогрев передних сидений Подогрев руля Подогрев форсунок стеклоомывателя Боковые зеркала с электрорегулировкой Боковые зеркала с обогревом Датчик света Стеклоподъёмник водителя с функцией Auto (вверх/вниз) Климат-контроль Круиз-контроль 8,0-дюймовый цветной сенсорный дисплей мультимедийной системы Apple CarPlay и Android Auto Дополнительные разъёмы зарядки USB Bluetooth для подключения мобильных устройств Распродажа склада Kia с пробегом до конца этой недели в Прагматика Купчино на ул. Малая Балканская, д.57. Сертифицированные автомобили Kia на гарантии с небольшим пробегом - отличная альтернатива новому автомобилю. Успейте купить с максимальной выгодой в городе. Центр проверенных автомобилей Прагматика Эксперт это Ваша гарантия безопасной покупки автомобиля, и полный спектр услуг, связанных с покупкой, страхованием и обслуживанием автомобиля в одной месте. Все для покупки автомобиля с пробегом “под ключ”: ✔️Только проверенные авто с пробегом ✔️Прозрачная история авто ✔️Юридическая безопасность сделки ✔️Предпродажная подготовка ✔️Большой выбор программ страхования: ОСАГО, ДАГО, КАСКО под разные задачи и бюджет ✔️Специальные сниженные цены за покупку в кредит ✔️Кредитные программы и возможность рассрочки (более 20 банков-партнеров) ✔️Ваш автомобиль может быть принят в качестве первоначального взноса. ✔️TRADE IN с выгодой до 100 000 руб. ✔️Срочный выкуп и возможность комиссионной продажи ✔️Установка доп. оборудования и постгарантийное обслуживание Прагматика Эксперт - крупная сеть автосалонов, представленная в городах: Санкт-Петербург, Великий Новгород, Псков, Великие Луки, Петрозаводск, Мурманск. Общий склад автомобилей с пробегом более 800 а/м. Посмотреть весь склад Вы можете на нашем сайте. Ищите нас по запросу pragmaticar.</t>
         </is>
       </c>
       <c r="AD3" t="inlineStr">
         <is>
-          <t>Luxe</t>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t>55000 км</t>
+        </is>
+      </c>
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t>Classic, Comfort, Luxe, Prestige, Style, Edition Plus</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Toyota Camry, 2022</t>
+          <t>Subaru XV, 2011</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>Subaru</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Camry</t>
+          <t>XV</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>сегодня в 16:01</t>
+          <t>сегодня в 17:43</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>от 3 850 000</t>
+          <t>1 199 000</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Пермский край, Пермь, ул. Спешилова, 111/3</t>
+          <t>Санкт-Петербург, Пушкинский р-н, пос. Шушары, Пулковское ш., 70</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://www.avito.ru/perm/avtomobili/toyota_camry_2022_2687747798</t>
+          <t>https://www.avito.ru/sankt-peterburg/avtomobili/subaru_xv_2011_3122339656</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2011</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>XV70 рестайлинг (2020—2023)</t>
+          <t>GP (2011—2016)</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -917,12 +962,12 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2.5 AT (204 л.с.)</t>
+          <t>1.6 4WD CVT (114 л.с.)</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>2.5 л</t>
+          <t>1.6 л</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
@@ -932,22 +977,22 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>Автомат</t>
+          <t>Вариатор</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Передний</t>
+          <t>Полный</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>Седан</t>
+          <t>Внедорожник 5-дверный</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Белый</t>
+          <t>Чёрный</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
@@ -962,94 +1007,99 @@
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>8,3 л/100 км</t>
+          <t>7,3 л/100 км</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>9,9 с</t>
+          <t>13,8 с</t>
         </is>
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>4885 мм</t>
+          <t>4450 мм</t>
         </is>
       </c>
       <c r="W4" t="inlineStr">
         <is>
-          <t>1455 мм</t>
+          <t>1570 мм</t>
         </is>
       </c>
       <c r="X4" t="inlineStr">
         <is>
-          <t>155 мм</t>
-        </is>
-      </c>
-      <c r="Y4" t="inlineStr">
-        <is>
-          <t>1590 мм</t>
-        </is>
-      </c>
-      <c r="Z4" t="inlineStr">
-        <is>
-          <t>1610 мм</t>
+          <t>220 мм</t>
         </is>
       </c>
       <c r="AA4" t="inlineStr">
         <is>
-          <t>3722***</t>
+          <t>JF1G*************</t>
         </is>
       </c>
       <c r="AC4" t="inlineStr">
         <is>
-          <t>УЖЕ В КЛЮЧАВТО ПЕРМЬ! НОВЫЕ АВТОМОБИЛИ ЛЮБИМЫХ БРЕНДОВ В НАЛИЧИИ! Для Вас:🔹специальные условия при покупке в кредит или по программе трейд-ин🔹гарантия дилера 2 года🔹выгодные кредиты! Более 30 банков партнеров Звоните уже сейчас! Менеджеры отдела продаж подробно проконсультируют по наличию возможных моделей и комплектаций.КЛЮЧАВТО – крупнейший автомобильный холдинг России и многократный победитель в номинации «Автодилер года» по версии Автостат🏆———————————————————————————ФУНКЦИОНАЛЬНОЕ ОБОРУДОВАНИЕ———————————————————————————• Центральный замок• Интеллектуальная система доступа в автомобиль Smart Entry• Светодиодные фары ближнего и дальнего света• Светодиодные передние противотуманные фары• Светодиодные дневные ходовые огни• Датчик света• Подогрев боковых зеркал заднего вида• Боковые зеркала заднего вида с электроприводом регулировки и складывания• Передние и задние электростеклоподъемники с функцией Auto• Электропривод регулировки водительского сиденья в 8 направлениях• Сиденье водителя с электрорегулировкой поясничной опоры в 2 направлениях• Электрорегулировка пассажирского сиденья в 4 направлениях, функция электрической регулировки с заднего сиденья• Электроусилитель рулевого управления (EPS)• Регулировка рулевой колонки по вылету и наклону• Мультифункциональное рулевое колесо• 2-зонный климат-контроль• Отдельная система кондиционирования для пассажиров: нет• Сегментированная панорамная крыша (открывающаяся, с защитой от защемления)• Антенна "Плавник акулы"• Мультимедийная система , 10-дюймовый дисплей• Аудиосистема с 6 динамиками• USB разъем для воспроизведения медиафайлов• 2 USB разъема для зарядки мобильных устройств пассажиров второго ряда• Коммуникационная система Bluetooth©• Задние датчики парковки• Сиденья второго ряда, складывающиеся в пропорции 60/40• 12.3-дюймовый цветной многофункциональный дисплей на панели приборов• 10-дюймовый цветной проекционный дисплей на лобовом стекле• Индикатор низкого уровня омывающей жидкости• Кнопки выбора режимов движения ECO/NORMAL/SPORT• Навигационная система• Круиз-контроль с функцией поддержания безопасной дистанции до впереди идущего автомобиля (DRCC)• Запуск двигателя кнопкой Push Start• Датчик дождя• Полностью светодиодные задние фонари• Автоматический корректор фар головного света• Электрохромное зеркало заднего вида• Ионизатор воздуха Nano-e———————————————————————————БЕЗОПАСНОСТЬ———————————————————————————• 2 фронтальные, 2 передние боковые и 2 задние боковые подушки безопасности• 2 шторки безопасности• 2 передние коленные подушки безопасности• Антиблокировочная система (ABS)• Система курсовой устойчивости (VSC)• Усилитель экстренного торможения (BA)• Электронное распределение тормозных усилий (EBD)• Антипробуксовочная система (TRC)• Система помощи при подъеме по склону (HAC)• Система контроля отклонения от полосы движения (LTA)• Система предупреждения об угрозе фронтального столкновения с функцией автоматического торможения и распознаванием пешеходов (PCS)• Система автоматической регулировки дальнего света фар (AHB)• Система мониторинга давления в шинах (TPMS)• Камера заднего вида с динамическими линиями разметки• Электромеханический стояночный тормоз (EPB)• Крепления ISOFIX для детских автокресел• Иммобилайзер———————————————————————————ИНТЕРЬЕР———————————————————————————• Цвет обивки сидений: черный• Цвет передней панели: черный• Цвет коврового покрытия: черный• Цвет потолка: серый• Количество мест: 5• Тип сидений: обычные• Салон: обивка сидений кожей• Рулевое колесо с кожаной обивкой• Кожаная обивка селектора управления трансмиссией• Металлические накладки на пороги• Подсветка органов управления, дверных ручек, перчаточного ящика, зоны ног водителя и переднего пассажира• Комплект ковриков салона класса люкс• Дополнительные воздуховоды для второго ряда сидений• Стекло с защитой от ультрафиолета• Переднее ветровое стекло и боковые передние стекла с шумоизоляцией———————————————————————————ЭКСТЕРЬЕР———————————————————————————• Белый Pearl• Тип кузова: седан• Количество дверей: 4• Легкосплавные колесные диски• Размер дисков: R18• Наружные ручки дверей, окрашенные в цвет кузова• Хромированные молдинги подоконной линии• Боковые зеркала заднего вида, окрашенные в цвет кузова• Нижняя решетка радиатора цвета тёмно-серый металлик• Неполноразмерное запасное колесо• Шины 235/45R18• Левая и правая круглые выхлопные трубы________* Дополнительные заводские опции.Место осмотраОсмотреть автомобиль можно по адресу: Пермь, ул. Спешилова, д. 111/3Комплектация «Deluxe»:Активная безопасность:Антиблокировочная системаАнтипробуксовочная системаСистема курсовой устойчивостиСистема помощи при экстренном торможенииСистема предотвращения столкновенияДатчик давления в шинахПассивная безопасность:Подушки безопасности водителяПодушки безопасности пассажираБоковые передние подушки безопасностиСистема крепления детских автокреселПротивоугонная система:ИммобилайзерЦентральный замокПомощь при вождении:Бортовой компьютерКруиз-контрольПарктроник заднийСистема помощи при старте в горуСистема контроля за полосой движенияСистема управления дальним светомДатчик светаДатчик дождяКомфорт:Усилитель руляЗапуск двигателя с кнопкиСистема доступа без ключаРегулировка руляЭлектрорегулировка сиденья водителяЭлектростеклоподъемники передниеЭлектропривод зеркалУправление климатом и обогрев:Климат-контроль 1-зонныйОбогрев зеркалМультимедиа и навигация:Навигационная системаМультифункциональное рулевое колесоСалон и интерьер:Темный салонКожаный рульПанорамная крышаСкладывающееся заднее сидениеЭкстерьер:Литые легкосплавные дискиРазмер дисков 18″Освещение:Светодиодные фарыПротивотуманные фарыАдаптивные фарыАвтоматический корректор фар</t>
+          <t>• Быстрый выкуп вашего автомобиля: - Выкупаем по рыночной стоимости; - Выкуп в день обращения; - Возможен выкуп кредитного автомобиля; - Специальные условия по программе «Trade-in», обменяем ваш старый авто на новый за 1 час. • Комиссионная продажа вашего автомобиля по вашей цене на условиях бесплатной стоянки. • Рефинансируем ваш автокредит под минимальную процентную ставку. _______________________________________________ Автомобиль представлен официальным дилером Чери Центр Пулково. Покупка в Чери Центр Пулково - это всегда проверенный автомобиль и целый ряд преимуществ: Мы предоставляем бесплатное такси от ст. м. Московский проспект до нашего автоцентра! • ГАРАНТИЯ ЮРИДИЧЕСКОЙ ЧИСТОТЫ: Мы осуществили все необходимые проверки и даём гарантию юридической чистоты всех наших автомобилей. • СТРАХОВАНИЕ КАСКО, ОСАГО: В нашем автоцентре Вы всегда можете осуществить любой вид автострахования. • ТЕХНИЧЕСКАЯ ДИАГНОСТИКА: Мы проверили состояние всех наших автомобилей по 56 пунктам, и предоставляем год гарантии на основные технические узлы. (Со всеми результатами диагностики Вы можете подробнее ознакомиться по телефону либо запросить документы непосредственно в автосалоне) Мы расскажем вам всю правду о состоянии автомобиля. • ПРЕДПРОДАЖНАЯ ПОДГОТОВКА: Мы произвели глубокую химчистку салона и полировку всех кузовных элементов, подготовили автомобиль для дальнейшей эксплуатации. • СПЕЦИАЛЬНЫЕ УСЛОВИЯ ПРИ ПОКУПКЕ АВТОМОБИЛЯ В КРЕДИТ: Предоставляется дополнительная скидка до 150 000 рублей.* • "TRADE-IN" Вашего авто - на представленный в нашей компании. При обмене Вашего автомобиля, также предоставляет дополнительные скидки до 150 000 рублей*. • ОГРОМНЫЙ ВЫБОР ДОПОЛНИТЕЛЬНОГО ОБОРУДОВАНИЯ: У нас вы сможете приобрести дополнительное оборудование на ваш автомобиль (защитные плёнки и покрытия, шины и диски, парктроник, сигнализацию и др. аксессуары). • ТЕСТ-ДРАЙВ: Мы всегда стремимся подобрать для Вас идеальный вариант, поэтому у нас возможно осуществить пробную поездку на любом понравившемся Вам автомобиле. ______________________________________________ • ПРЕИМУЩЕСТВА АВТОКРЕДИТОВАНИЯ: ✓ Автокредит без страховых нагрузок; ✓ По двум документам (паспорт РФ, водительское удостоверение); ✓ Первоначальный взнос от 0%; ✓ Ставка по автокредиту от 7,9%; ✓ Более 15 банков партнеров; ✓ Более 52 различных программ; ✓ Автокредит до 3 000 000 рублей; ✓ Возможность досрочного погашения без комиссий и штрафов. Подача заявки также доступна онлайн: просто позвоните, и кредитный специалист проконсультирует Вас! Если наш автомобиль вас не заинтересовал, то мы поможем вам приобрести любой другой автомобиль в кредит через наш автосалон. Ждём Вас ежедневно с 9 до 21 по адресу: г. Санкт-Петербург, Пулковское шоссе, д. 70 Местонахождение нашего автоцентра на карте вы можете увидеть на последнем фото.  *Данные скидки применяются в зависимости от условий покупки, а также от цены автомобиля.</t>
+        </is>
+      </c>
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="AE4" t="inlineStr">
+        <is>
+          <t>108802 км</t>
+        </is>
+      </c>
+      <c r="AF4" t="inlineStr">
+        <is>
+          <t>Base, BL, CC, DE, NAV, PC, S/AB</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ВАЗ (LADA) Granta, 2023</t>
+          <t>Mitsubishi Outlander, 2016</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ВАЗ</t>
+          <t>Mitsubishi</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>(LADA)</t>
+          <t>Outlander</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>сегодня в 16:21</t>
+          <t>сегодня в 17:45</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>от 656 900</t>
+          <t>1 399 000</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Пермский край, Пермь, Пушкарская ул., 138</t>
+          <t>Санкт-Петербург, пр-т Маршала Жукова, 51</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>https://www.avito.ru/perm/avtomobili/vaz_lada_granta_2023_3162673418</t>
+          <t>https://www.avito.ru/sankt-peterburg/avtomobili/mitsubishi_outlander_2016_3022274188</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>2016</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>I рестайлинг (2018—2023)</t>
+          <t>III рестайлинг 2 (2015—2018)</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -1059,12 +1109,12 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>1.6 MT (90 л.с.)</t>
+          <t>2.0 4WD CVT (146 л.с.)</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>1.6 л</t>
+          <t>2.0 л</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
@@ -1074,22 +1124,22 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>Механика</t>
+          <t>Вариатор</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Передний</t>
+          <t>Полный</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>Седан</t>
+          <t>Внедорожник 5-дверный</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Чёрный</t>
+          <t>Серый</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
@@ -1099,99 +1149,114 @@
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>0 л</t>
+          <t>60 л</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>6,8 л/100 км</t>
+          <t>7,7 л/100 км</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>11,2 с</t>
+          <t>12 с</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>4268 мм</t>
+          <t>4695 мм</t>
         </is>
       </c>
       <c r="W5" t="inlineStr">
         <is>
-          <t>1500 мм</t>
+          <t>1680 мм</t>
         </is>
       </c>
       <c r="X5" t="inlineStr">
         <is>
-          <t>180 мм</t>
+          <t>215 мм</t>
         </is>
       </c>
       <c r="Y5" t="inlineStr">
         <is>
-          <t>1430 мм</t>
+          <t>1540 мм</t>
         </is>
       </c>
       <c r="Z5" t="inlineStr">
         <is>
-          <t>1418 мм</t>
+          <t>1540 мм</t>
         </is>
       </c>
       <c r="AA5" t="inlineStr">
         <is>
-          <t>XTA2*************</t>
+          <t>Z8TX*************</t>
         </is>
       </c>
       <c r="AC5" t="inlineStr">
         <is>
-          <t>💥LADA по цене от завода в Брайт Парке! Доп. оборудование в подарок 💥 🔥 АКЦИЯ - УТИЛИЗАЦИЯ 🔥 ТОЛЬКО В ИЮНЕ по программе Утилизации выкупим ваш старый автомобиль за 160 000 рублей. Используйте их как первоначальный взнос при покупке своей новой LADA Дополнительно: ✅ ЛЁГКИЙ КРЕДИТ • Гибкие кредитные программы, возможность купить автомобиль без КАСКО/Страхования жизни • Более 20 банков партнеров • Первоначальный взнос от 0% • Ваш автомобиль может стать первоначальным взносом ✅ МОЩНЫЙ ОБМЕН • Оценка авто по рыночной цене • Бесплатная диагностика • Выкупаем залоговые автомобили ✅НАШИ ПРЕИМУЩЕСТВА • Склад автомобилей с ПТС • Возможность уехать на новом автомобиле день в день Официальный дилер LADA с 2014 года Наша команда профессионалов сделает для вас приобретение автомобиля комфортным и быстрым. .</t>
+          <t>Код автомобиля: Ю-158. Автомобиль принят по программе Trade In. Проведена комплексная техническая диагностика. Отличное техническое и внешнее состояние. Два владельца. Комплектация : - кожаный салон - климат-контроль - электропривод и подогрев зеркал - электропривод складывания боковых зеркал - ABS/ESP/ Bluetooth - противотуманные фары - подогрев передних сидений - аудиосистема с управлением на руле - круиз-контроль - камера заднего вида - бесключевой доступ в автомобиль - запуск двигателя с кнопки - датчики дождя/света - легкосплавные диски - электропривод крышки багажника - иммобилайзер - крепление для детского кресла (isofix/latch) Возможна продажа в кредит. Возможен обмен на Ваш автомобиль. ДЦ «Аларм-Моторс Юго-Запад». Проспект Маршала Жукова д.51.</t>
+        </is>
+      </c>
+      <c r="AD5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AE5" t="inlineStr">
+        <is>
+          <t>190000 км</t>
+        </is>
+      </c>
+      <c r="AF5" t="inlineStr">
+        <is>
+          <t>Instyle, Intense, Intense+, Invite</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Renault Sandero Stepway, 2022</t>
+          <t>Volkswagen Jetta, 2017</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Renault</t>
+          <t>Volkswagen</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Sandero</t>
+          <t>Jetta</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>сегодня в 16:04</t>
+          <t>сегодня в 18:06</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>от 1 730 544</t>
+          <t>890 000</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Пермский край, Пермь, Подлесная ул., 47А</t>
+          <t>Санкт-Петербург, 2 линия</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>https://www.avito.ru/perm/avtomobili/renault_sandero_stepway_2022_3234511269</t>
+          <t>https://www.avito.ru/sankt-peterburg/avtomobili/volkswagen_jetta_2017_3087029920</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2017</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>II рестайлинг (2018—2023)</t>
+          <t>VI рестайлинг (2014—2019)</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -1201,12 +1266,12 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>1.6 CVT (113 л.с.)</t>
+          <t>1.4 TSI DSG (125 л.с.)</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>1.6 л</t>
+          <t>1.4 л</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
@@ -1216,7 +1281,7 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>Вариатор</t>
+          <t>Робот</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
@@ -1226,12 +1291,12 @@
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>Хетчбек 5-дверный</t>
+          <t>Седан</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Синий</t>
+          <t>Серый</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -1246,54 +1311,69 @@
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>6,7 л/100 км</t>
+          <t>5,7 л/100 км</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>11,9 с</t>
+          <t>9,6 с</t>
         </is>
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>4083 мм</t>
+          <t>4659 мм</t>
         </is>
       </c>
       <c r="W6" t="inlineStr">
         <is>
-          <t>1626 мм</t>
+          <t>1482 мм</t>
         </is>
       </c>
       <c r="X6" t="inlineStr">
         <is>
-          <t>195 мм</t>
+          <t>160 мм</t>
         </is>
       </c>
       <c r="Y6" t="inlineStr">
         <is>
-          <t>1497 мм</t>
+          <t>1535 мм</t>
         </is>
       </c>
       <c r="Z6" t="inlineStr">
         <is>
-          <t>1486 мм</t>
+          <t>1538 мм</t>
         </is>
       </c>
       <c r="AA6" t="inlineStr">
         <is>
-          <t>X7L5*************</t>
-        </is>
-      </c>
-      <c r="AC6" t="inlineStr">
-        <is>
-          <t>⚡Новый Renault за наличные или в кредитОграниченное количество автомобилей в ПермиЗаберите свой Renault прямо сегодня------------------------Компания САТУРН-Р-АВТО представляет только актуальный склад автомобилей в наличии.✅Мы указываем только реальные условия покупки✅Мы заберем Ваш старый автомобиль и сделаем скидку на новый по программе трейд-ин.✅В наличии всегда большой выбор комплектаций и расцветок автомобилей ✅Выгодные кредитные программы со сниженной ставкой от 17 банков.✅Доступные программы автострахования КАСКО и ОСАГО от 26 страховых компаний.✅Гарантия на автомобиль 3 ГОДА или 100 000 км пробега в зависимости от того, что наступит ранее.☎️Звоните прямо сейчас и бронируйте ваш Renault в САТУРН-Р-АВТО------------------------САТУРН-Р-АВТО - новые автомобили Renault в Перми Пермь, Подлесная, 47А* Цена автомобиля может быть увеличена на сумму установленного дополнительного оборудования. Кредитор ПАО «Росбанк», лицензия ЦБ РФ № 2272 от 28.01.2015 г. Предложение распространяется на новые автомобили RenaultПредставленное изображение носит информационный характер, может отличаться от реального товара. Не оферта. Предложение ограничено, подробности уточняйте у менеджеров отдела продаж.</t>
+          <t>XW8Z*************</t>
+        </is>
+      </c>
+      <c r="AB6" t="inlineStr">
+        <is>
+          <t>Оригинал</t>
+        </is>
+      </c>
+      <c r="AD6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AE6" t="inlineStr">
+        <is>
+          <t>112430 км</t>
+        </is>
+      </c>
+      <c r="AF6" t="inlineStr">
+        <is>
+          <t>Life, Trendline, Allstar, Comfortline, Highline</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Kia K5, 2023</t>
+          <t>Kia Sportage, 2020</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1303,37 +1383,37 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>K5</t>
+          <t>Sportage</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>сегодня в 15:50</t>
+          <t>сегодня в 17:51</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>3 119 900</t>
+          <t>2 370 000</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Пермский край, Березники, Березниковская ул., 35</t>
+          <t>Санкт-Петербург, Балтийский б-р, 4</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>https://www.avito.ru/berezniki/avtomobili/kia_k5_2023_3242166703</t>
+          <t>https://www.avito.ru/sankt-peterburg/avtomobili/kia_sportage_2020_3251955560</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>2020</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>III (2019—2023)</t>
+          <t>IV рестайлинг (2018—2023)</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -1343,7 +1423,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2.0 MPI AT (150 л.с.)</t>
+          <t>2.0 MPI 4WD AT (150 л.с.)</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
@@ -1363,17 +1443,17 @@
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Передний</t>
+          <t>Полный</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Седан</t>
+          <t>Внедорожник 5-дверный</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Серый</t>
+          <t>Красный</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -1383,109 +1463,114 @@
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>70 л</t>
+          <t>62 л</t>
         </is>
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>7,2 л/100 км</t>
+          <t>8,3 л/100 км</t>
         </is>
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>10,6 с</t>
+          <t>11,6 с</t>
         </is>
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>4905 мм</t>
+          <t>4485 мм</t>
         </is>
       </c>
       <c r="W7" t="inlineStr">
         <is>
-          <t>1465 мм</t>
+          <t>1655 мм</t>
         </is>
       </c>
       <c r="X7" t="inlineStr">
         <is>
-          <t>155 мм</t>
+          <t>182 мм</t>
         </is>
       </c>
       <c r="Y7" t="inlineStr">
         <is>
-          <t>1618 мм</t>
+          <t>1625 мм</t>
         </is>
       </c>
       <c r="Z7" t="inlineStr">
         <is>
-          <t>1625 мм</t>
+          <t>1636 мм</t>
         </is>
       </c>
       <c r="AA7" t="inlineStr">
         <is>
-          <t>MX1G*************</t>
+          <t>XWEP*************</t>
         </is>
       </c>
       <c r="AB7" t="inlineStr">
         <is>
-          <t>Электронный</t>
-        </is>
-      </c>
-      <c r="AC7" t="inlineStr">
-        <is>
-          <t>В KIA Центр Березники в наличии автомобили KIA на выгодных условиях! Гарантия на автомобиль 2 года или 60 тыс. км. Ждём Вас в KIA Центр Березники по адресу: г. Березники, ул. Березниковская, 35 *Фото носит информационный характер Скидки от дилера  3 319 900 ₽Цена без скидки 100 000 ₽За трейд-ин 100 000 ₽За кредит 200 000 ₽Максимальная скидка  Со всеми скидками 3 119 900 ₽ Свяжитесь с дилером, чтобы узнать условия предоставления скидок. __________________________________________________________ Официальный дилер KIA Центр Березники – это лучшее место для выбора нового автомобиля KIA! · С нами УДОБНО! Выбрав нас в качестве официального дилера KIA, Вам не придется ждать автомобиль неделями, в нашем автоцентре представлен весь модельный ряд. · С нами ВЫГОДНО! Вы будете приятно удивлены впечатляющими выгодами и гарантированными подарками на автомобили KIA при любых условиях приобретения! · С нами ПРОСТО! Воспользовавшись услугой Trade-in, Вы отдаете свой автомобиль по высокой рыночной цене в зачет нового KIA, снимая с себя необходимость решения хлопотных вопросов. · С нами БЫСТРО! Каждый автомобиль сопровождается оригиналом ПТС, что позволит оформить автомобиль в кратчайшие сроки! · С нами СПОКОЙНО! Ведущие банки России одобрят Вам кредит за 15 минут на лучших условиях. · С нами НАДЕЖНО! Команда профессионалов всегда предложит лучшие персональные условия, поможет в оформлении кредита и выкупе Вашего автомобиля.</t>
+          <t>Оригинал</t>
         </is>
       </c>
       <c r="AD7" t="inlineStr">
         <is>
-          <t>Comfort</t>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AE7" t="inlineStr">
+        <is>
+          <t>109000 км</t>
+        </is>
+      </c>
+      <c r="AF7" t="inlineStr">
+        <is>
+          <t>Comfort, Luxe, Prestige, Luxe+, UEFA Europa League, Edition Plus, Prestige Black Edition</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Hyundai Santa Fe, 2022</t>
+          <t>Land Rover Range Rover Velar, 2018</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Hyundai</t>
+          <t>Land</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Santa</t>
+          <t>Rover</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>сегодня в 15:58</t>
+          <t>сегодня в 17:48</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>4 372 000</t>
+          <t>4 279 000</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Пермский край, Пермь, ул. Спешилова, 109</t>
+          <t>Санкт-Петербург, Выборгское ш., 27к2Б</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>https://www.avito.ru/perm/avtomobili/hyundai_santa_fe_2022_2169048931</t>
+          <t>https://www.avito.ru/sankt-peterburg/avtomobili/land_rover_range_rover_velar_2018_2396365531</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2018</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>IV рестайлинг (2020—2023)</t>
+          <t>I (2017—2023)</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -1495,17 +1580,17 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2.5 4WD AT (180 л.с.)</t>
+          <t>D180 2.0 AT (180 л.с.)</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>2.5 л</t>
+          <t>2.0 л</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>Бензин</t>
+          <t>Дизель</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
@@ -1525,7 +1610,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Чёрный</t>
+          <t>Серый</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -1535,109 +1620,114 @@
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>67 л</t>
+          <t>60 л</t>
         </is>
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>8,7 л/100 км</t>
+          <t>5,4 л/100 км</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>10,3 с</t>
+          <t>8,9 с</t>
         </is>
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>4785 мм</t>
+          <t>4803 мм</t>
         </is>
       </c>
       <c r="W8" t="inlineStr">
         <is>
-          <t>1685 мм</t>
+          <t>1665 мм</t>
         </is>
       </c>
       <c r="X8" t="inlineStr">
         <is>
-          <t>205 мм</t>
+          <t>213 мм</t>
         </is>
       </c>
       <c r="Y8" t="inlineStr">
         <is>
-          <t>1637 мм</t>
+          <t>1642 мм</t>
         </is>
       </c>
       <c r="Z8" t="inlineStr">
         <is>
-          <t>1647 мм</t>
+          <t>1657 мм</t>
         </is>
       </c>
       <c r="AA8" t="inlineStr">
         <is>
-          <t>XWES*************</t>
-        </is>
-      </c>
-      <c r="AB8" t="inlineStr">
-        <is>
-          <t>Оригинал</t>
+          <t>SALY*************</t>
         </is>
       </c>
       <c r="AC8" t="inlineStr">
         <is>
-          <t>СИЛЬВЕР МОТОРС – официальный дилер HYUNDAI в Камской долине предлагает выгодные условия на покупку нового автомобиля!  HYUNDAI SANTA FE в комплектации FAMILY по специальной цене! Стоимость автомобиля без учета скидок от дилера    Максимальная выгода по трейд-ин, возможность рассрочки и низкая процентная ставка! Не упустите шанс выгодно купить долгожданный автомобиль HYUNDAI перед повышением цен. Звоните прямо сейчас! Менеджер ответит на все ваши вопросы!  Более 15 лет мы работаем над тем, чтобы качественные и комфортные автомобили HYUNDAI принадлежали именно вам! Стараемся предоставлять вам достойный сервис, делать выгодные предложения и скидки, полностью помогать в выборе автомобиля, следуя вашим потребностям. Не пропустите спецпредложения в СИЛЬВЕР МОТОРС на покупку нового автомобиля:  - HYUNDAI без первоначального взноса на весь модельный ряд. Первоначальный взнос 0%! Позвольте себе больше!  - Хотите приобрести новый автомобиль, но еще не выплатили кредит за свой нынешний автомобиль? Наша программа «Ключ за ключ» позволит сделать это быстро и комфортно!  ***Предложение не является официальной офертой. Стоимость актуальна на момент публикации с учетом всех спецпредложений. Фото носит информационный характер.  __________________________________________________________  В наших салонах вы всегда можете воспользоваться дополнительными услугами:  • обменять свой старый автомобиль на новый по программе трейд-ин  • оформить выгодный кредит  • надежно застраховать автомобиль  • пройти сервисное обслуживание вашего автомобиля  • выбрать, продать или обменять авто с пробегом  • наши актуальные акции  __________________________________________________________</t>
+          <t>Купить автомобиль с пробегом у официального дилера «Форсаж» Volkswagen, УАЗ, HAVAL— это безопасно, быстро и комфортно.⭐ЧЕСТНАЯ ЦЕНА - цена без скрытых условий, за наличный расчет⭐⭐Оригинал ПТС⭐Оригинальный пробег⭐1 Собственник⭐Отличное внешнее и техническое состояние✅Честная процентная ставка по кредиту от 9,5% годовых ✅Кредиты с временной регистрацией✅Кредит ПЛАТИ МЕНЬШЕ: кредит с остаточным платежом✅Кредит без первоначального взноса!✅ Кредитование от 12 месяцев до 96 месяцев (8 лет)✅Уровень одобрений 95%✅Покупка авто одним днём Для кредита:❕Нужен только паспорт❕ ✔95% одобрений✔🔹Сотрудничаем с 1️⃣7️⃣ надежными банками🔹🚘Форсаж🚘 Почему именно мы?📍Выгодные условия приобретения📍Предпродажная подготовка📍Гарантия юридической чистоты. Наши эксперты проводят сверку номерных агрегатов📍Предоставление полного пакета документов для регистрации автомобиля в органах ГИБДД📍Проверенные автомобили с пробегом, прошедшие полную комплексную техническую диагностику📍Специальные предложения на сервисное обслуживание и дополнительное оборудование📍Уникальное предложение по кредиту от банков-партнеров📍Примем ваш авто в зачет с выгодой до 30 000р📞Пишите и звоните прямо сейчас! Рады видеть Вас каждый день с 9 до 21 по адресу: Выборгское шоссе, 27 к2БПТС оригинал.Место осмотраОсмотреть автомобиль можно по адресу: Санкт-Петербург, Выборгское шоссе 27, Volkswagen Форсаж ОзеркиКомплектация «R-Dynamic S»:Активная безопасность:Антиблокировочная системаСистема курсовой устойчивостиДатчик давления в шинахПассивная безопасность:Подушки безопасности водителя с защитой коленейПодушки безопасности пассажираБоковые передние подушки безопасностиОконные шторки безопасностиБлокировка замков задних дверейСистема крепления детских автокреселПротивоугонная система:Датчик проникновения в салон (датчик объема)ИммобилайзерЦентральный замокПомощь при вождении:Бортовой компьютерКруиз-контрольПарктроник заднийКамера заднего видаСистема помощи при старте в горуДатчик светаДатчик дождяКомфорт:Активный усилитель руляЗапуск двигателя с кнопкиСистема доступа без ключаРегулировка руляЭлектрорегулировка сиденья пассажира с памятью положенияЭлектростеклоподъемники передние и задниеЭлектропривод зеркалЭлектропривод крышки багажникаУправление климатом и обогрев:Климат-контроль 1-зонныйПодогрев руляОбогрев зеркалОбогрев лобового стеклаПрограммируемый предпусковой отопительМультимедиа и навигация:Навигационная системаCDUSBГолосовое управлениеBluetoothAUXАудиоподготовкаМультифункциональное рулевое колесоРозетка 12VСалон и интерьер:Кожаная обивка салонаКожаный рульСкладывающееся заднее сидениеТретий задний подголовникПередний центральный подлокотникПодрулевые лепестки переключения передачМеталлические накладки на педалиНакладки на порогиЭкстерьер:Литые легкосплавные дискиРазмер дисков 19″Задние тонированные стеклаЗащита картераДекоративные молдингиОсвещение:Светодиодные фарыАвтоматический корректор фарОмыватель фарКомплектность:Сервисная книжкаОтметки ТО ВсеПТССвидетельство о регистрации2 комплекта ключейКомплект резиновых ковриков</t>
         </is>
       </c>
       <c r="AD8" t="inlineStr">
         <is>
-          <t>Family 5 мест</t>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AE8" t="inlineStr">
+        <is>
+          <t>44404 км</t>
+        </is>
+      </c>
+      <c r="AF8" t="inlineStr">
+        <is>
+          <t>Base, R-Dynamic Base, R-Dynamic S, R-Dynamic SE, S, SE</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Hyundai Palisade, 2022</t>
+          <t>Skoda Octavia, 2015</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Hyundai</t>
+          <t>Skoda</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Palisade</t>
+          <t>Octavia</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>сегодня в 14:01</t>
+          <t>сегодня в 17:46</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>5 900 000</t>
+          <t>1 019 000</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Пермский край, Пермь, ул. Героев Хасана, 76</t>
+          <t>Санкт-Петербург, Дунайский пр-т, 25к3</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>https://www.avito.ru/perm/avtomobili/hyundai_palisade_2022_3094526020</t>
+          <t>https://www.avito.ru/sankt-peterburg/avtomobili/skoda_octavia_2015_3047225980</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>I рестайлинг (2022—2023)</t>
+          <t>III (2013—2017)</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -1647,37 +1737,37 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2.2 CRDi 4WD AT (202 л.с.)</t>
+          <t>1.4 TSI MT (140 л.с.)</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>2.2 л</t>
+          <t>1.4 л</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>Дизель</t>
+          <t>Бензин</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>Автомат</t>
+          <t>Механика</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Полный</t>
+          <t>Передний</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>Внедорожник 5-дверный</t>
+          <t>Лифтбек</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>Белый</t>
+          <t>Синий</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
@@ -1687,109 +1777,114 @@
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>71 л</t>
+          <t>0 л</t>
         </is>
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>8,5 л/100 км</t>
+          <t>5,5 л/100 км</t>
         </is>
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>10,5 с</t>
+          <t>8,4 с</t>
         </is>
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>4995 мм</t>
+          <t>4659 мм</t>
         </is>
       </c>
       <c r="W9" t="inlineStr">
         <is>
-          <t>1750 мм</t>
+          <t>1461 мм</t>
         </is>
       </c>
       <c r="X9" t="inlineStr">
         <is>
-          <t>203 мм</t>
+          <t>155 мм</t>
         </is>
       </c>
       <c r="Y9" t="inlineStr">
         <is>
-          <t>1708 мм</t>
+          <t>1549 мм</t>
         </is>
       </c>
       <c r="Z9" t="inlineStr">
         <is>
-          <t>1716 мм</t>
+          <t>1520 мм</t>
         </is>
       </c>
       <c r="AA9" t="inlineStr">
         <is>
-          <t>KMHR*************</t>
-        </is>
-      </c>
-      <c r="AB9" t="inlineStr">
-        <is>
-          <t>Электронный</t>
+          <t>XW8A*************</t>
         </is>
       </c>
       <c r="AC9" t="inlineStr">
         <is>
-          <t>________________________________________________  Особенности комплектации: • Беспроводное зарядное устройство (стандарт Qi) • Легкосплавные диски 20" с шинами 245/50R20 • Камера заднего вида с динамическими указателями траектории движения, Задние датчики парковки, Передние датчики парковки, Круговой обзор • Светодиодные фары • Система доступа в салон без ключа и кнопка запуска двигателя • Премиум-аудиосистема KRELL: 12 динамиков, вкл. сабвуфер, внешний усилитель • Интеграция со смартфонами (Apple CarPlay™/Android Auto™) • Вентиляция и подогрев передних сидений • Раздельные сиденья 2-го ряда (компоновка 2:2:3), вентиляция и подогрев сидений 2-го ряда • Подогрев сидений 3-го ряда • Датчик дождя и Датчик света • Автоматическое переключение ближний/дальний свет (HBA) • Электропривод двери багажника с системой автоматического открывания • Самозатемняющееся внутрисалонное зеркало • Система кругового обзора (SVM) • Система обзора слепых зон (BVM) • Цифровая приборная панель с диагональю 12,3” • Проекция показаний приборов на лобовое стекло • Электропривод подъема/складывания сидений третьего ряда • Память положения водительского сиденья, рулевого колеса, наружных зеркал заднего вида, положения показаний проекционного дисплея для двух водителей • Складывание спинки второго ряда сидений одним нажатием из багажника • Интеллектуальный круиз-контроль с функцией полной остановки и начала движения • Трехзонный климат-контроль • Остекление с дополнительной шумоизоляцией (лобовое и передние боковые стёкла) • Отделка потолка и стоек замшей • Отделка сидений кожей Nappa • Фонари заднего хода с проекцией на дорожное покрытие ________________________________________________   «ДАВ-АВТО» - официальный дилер HYUNDAI в Перми и Пермском крае. Находимся по адресу: г.Пермь, ул.Героев Хасана, д.76 ________________________________________________ Так же при покупке нового HYUNDAI в нашем дилерском центре «ДАВ-АВТО» Вы можете: · Получить специальные условия по автокредитованию · Обменять свой автомобиль на новый по программе Trade-In · Получить специальные условия по страхованию автомобиля · Пройти полное сервисное обслуживание Вашего автомобиля ________________________________________________ *Стоимость автомобиля указана с учётом специальных условий. *Автомобиль без пробега по РФ, не ставился на учёт в России.  Стоимость автомобиля с учетом скидок от дилера 5 900 000р. Скидка по программе Трейд-Ин 150 000 р Скидка по программе автокредитования 150 000 р Максимальная скидка 300 000 р. Стоимость автомобиля без учета скидок 6 200 000 р</t>
+          <t>ПТС оригинал.Место осмотраОсмотреть автомобиль можно по адресу: Санкт-Петербург, Дунайский проспект, дом 25/3, лит.АКомплектация:Активная безопасность:Антиблокировочная системаСистема курсовой устойчивостиПассивная безопасность:Подушки безопасности водителяПодушки безопасности пассажираСистема крепления детских автокреселПротивоугонная система:ИммобилайзерЦентральный замокПомощь при вождении:Бортовой компьютерСистема помощи при старте в горуКомфорт:Усилитель руляРегулировка руляЭлектростеклоподъемники передниеЭлектропривод зеркалУправление климатом и обогрев:Обогрев зеркалОбогрев форсунок стеклоомывателейМультимедиа и навигация:АудиоподготовкаСалон и интерьер:Тканевая обивка салонаСкладывающееся заднее сидениеПрикуриватель и пепельницаЭкстерьер:Штампованные стальные диски</t>
         </is>
       </c>
       <c r="AD9" t="inlineStr">
         <is>
-          <t>Базовая</t>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AE9" t="inlineStr">
+        <is>
+          <t>142336 км</t>
+        </is>
+      </c>
+      <c r="AF9" t="inlineStr">
+        <is>
+          <t>Базовая, Ambition, Elegance</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Hyundai Elantra, 2022</t>
+          <t>Datsun on-DO, 2015</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Hyundai</t>
+          <t>Datsun</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Elantra</t>
+          <t>on-DO</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>сегодня в 14:16</t>
+          <t>сегодня в 17:45</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2 990 000</t>
+          <t>419 000</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Пермский край, Пермь, ул. Героев Хасана, 76</t>
+          <t>Санкт-Петербург, пр-т Маршала Жукова, 51</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>https://www.avito.ru/perm/avtomobili/hyundai_elantra_2022_2902655285</t>
+          <t>https://www.avito.ru/sankt-peterburg/avtomobili/datsun_on-do_2015_3149743225</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>VII (2020—2023)</t>
+          <t>I (2014—2019)</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
@@ -1799,7 +1894,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>1.6 AT (128 л.с.)</t>
+          <t>1.6 MT (87 л.с.)</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
@@ -1814,7 +1909,7 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>Автомат</t>
+          <t>Механика</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
@@ -1829,7 +1924,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>Красный</t>
+          <t>Коричневый</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
@@ -1839,104 +1934,114 @@
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>47 л</t>
+          <t>0 л</t>
         </is>
       </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t>6,9 л/100 км</t>
+          <t>7 л/100 км</t>
         </is>
       </c>
       <c r="U10" t="inlineStr">
         <is>
-          <t>11,3 с</t>
+          <t>12,2 с</t>
         </is>
       </c>
       <c r="V10" t="inlineStr">
         <is>
-          <t>4650 мм</t>
+          <t>4336 мм</t>
         </is>
       </c>
       <c r="W10" t="inlineStr">
         <is>
-          <t>1430 мм</t>
+          <t>1500 мм</t>
         </is>
       </c>
       <c r="X10" t="inlineStr">
         <is>
-          <t>150 мм</t>
+          <t>174 мм</t>
         </is>
       </c>
       <c r="Y10" t="inlineStr">
         <is>
-          <t>1585 мм</t>
+          <t>1431 мм</t>
         </is>
       </c>
       <c r="Z10" t="inlineStr">
         <is>
-          <t>1596 мм</t>
+          <t>1426 мм</t>
         </is>
       </c>
       <c r="AA10" t="inlineStr">
         <is>
-          <t>KMHL*************</t>
-        </is>
-      </c>
-      <c r="AB10" t="inlineStr">
-        <is>
-          <t>Электронный</t>
+          <t>Z8NB*************</t>
         </is>
       </c>
       <c r="AC10" t="inlineStr">
         <is>
-          <t>На автомобиль действует скидка 10% от указанной стоимости по Г.О.С. программе. ________________________________________________  Особенности комплектации:  • Беспроводное зарядное устройство (стандарт Qi) • Легкосплавные диски 17" с шинами 225/45R17 • Камера заднего вида с динамическими указателями траектории движения, Задние датчики парковки, Передние датчики парковки • Светодиодные фары • Система доступа в салон без ключа и кнопка запуска двигателя • Премиальная аудиосистема Bose (8 динамиков включая сабвуфер) • Интеграция со смартфонами (Apple CarPlay™/Android Auto™) • Вентиляция передних сидений • Подогрев задних сидений • Датчик дождя и Датчик света • Автоматическое переключение ближний/дальний свет (HBA) • Крыша с люком • Электрорегулировки сиденья водителя + поясничная поддержка водителя • Самозатемняющееся внутрисалонное зеркало • Электрорегулировки сиденья переднего пассажира • Система обзора слепых зон (BVM) • Цифровая приборная панель 10,25" • Навигационная система с HD экраном 10,25" (Apple CarPlay™/Android Auto™1) • Комбинация натуральной и искусственной кожи в отделке сидений • Память настроек сиденья водителя (для двух водителей: сиденье, внешние зеркала) • Уникальный цвет салона: Светло-серый Меланж • Интеллектуальный круиз-контроль с функцией полной остановки и начала движения ________________________________________________   «ДАВ-АВТО» - официальный дилер HYUNDAI в Перми и Пермском крае. Находимся по адресу: г.Пермь, ул.Героев Хасана, д.76 ________________________________________________ Так же при покупке нового HYUNDAI в нашем дилерском центре «ДАВ-АВТО» Вы можете: · Получить специальные условия по автокредитованию · Обменять свой автомобиль на новый по программе Trade-In · Получить специальные условия по страхованию автомобиля · Пройти полное сервисное обслуживание Вашего автомобиля ________________________________________________ *Стоимость автомобиля указана с учётом специальных условий. *Автомобиль без пробега по РФ, не ставился на учёт в России.</t>
+          <t>Код автомобиля: Ю-25. Автомобиль принят по программе Trade In. Проведена комплексная техническая диагностика. ПТС оригинал. Один владелец. Комплектация : - зеркала с эл.регулировкой - аудиосистема - ABS - USB/AUX - стальные диски - противотуманные фары - крепление для детского кресла (isofix/latch) - подогрев передних сидений Возможна продажа в кредит. Возможен обмен на Ваш автомобиль. ДЦ «Аларм-Моторс Юго-Запад». Проспект Маршала Жукова д.51.</t>
+        </is>
+      </c>
+      <c r="AD10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AE10" t="inlineStr">
+        <is>
+          <t>128000 км</t>
+        </is>
+      </c>
+      <c r="AF10" t="inlineStr">
+        <is>
+          <t>Access, Dream I, Dream II, Trust I, Trust II, Trust III, Dream III, Trust, Comfort</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Hyundai Palisade, 2022</t>
+          <t>Kia Sportage, 2021</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Hyundai</t>
+          <t>Kia</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Palisade</t>
+          <t>Sportage</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>сегодня в 14:01</t>
+          <t>сегодня в 18:01</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>5 900 000</t>
+          <t>2 441 000</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Пермский край, Пермь, ул. Героев Хасана, 76</t>
+          <t>Санкт-Петербург, Ириновский пр-т, 10</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>https://www.avito.ru/perm/avtomobili/hyundai_palisade_2022_3094526020</t>
+          <t>https://www.avito.ru/sankt-peterburg/avtomobili/kia_sportage_2021_2891557072</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>I рестайлинг (2022—2023)</t>
+          <t>IV рестайлинг (2018—2023)</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -1946,17 +2051,17 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2.2 CRDi 4WD AT (202 л.с.)</t>
+          <t>2.0 MPI 4WD AT (150 л.с.)</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>2.2 л</t>
+          <t>2.0 л</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>Дизель</t>
+          <t>Бензин</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
@@ -1986,109 +2091,114 @@
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>71 л</t>
+          <t>62 л</t>
         </is>
       </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>8,5 л/100 км</t>
+          <t>8,3 л/100 км</t>
         </is>
       </c>
       <c r="U11" t="inlineStr">
         <is>
-          <t>10,5 с</t>
+          <t>11,6 с</t>
         </is>
       </c>
       <c r="V11" t="inlineStr">
         <is>
-          <t>4995 мм</t>
+          <t>4485 мм</t>
         </is>
       </c>
       <c r="W11" t="inlineStr">
         <is>
-          <t>1750 мм</t>
+          <t>1655 мм</t>
         </is>
       </c>
       <c r="X11" t="inlineStr">
         <is>
-          <t>203 мм</t>
+          <t>182 мм</t>
         </is>
       </c>
       <c r="Y11" t="inlineStr">
         <is>
-          <t>1708 мм</t>
+          <t>1625 мм</t>
         </is>
       </c>
       <c r="Z11" t="inlineStr">
         <is>
-          <t>1716 мм</t>
+          <t>1636 мм</t>
         </is>
       </c>
       <c r="AA11" t="inlineStr">
         <is>
-          <t>KMHR*************</t>
-        </is>
-      </c>
-      <c r="AB11" t="inlineStr">
-        <is>
-          <t>Электронный</t>
+          <t>XWEP*************</t>
         </is>
       </c>
       <c r="AC11" t="inlineStr">
         <is>
-          <t>________________________________________________  Особенности комплектации: • Беспроводное зарядное устройство (стандарт Qi) • Легкосплавные диски 20" с шинами 245/50R20 • Камера заднего вида с динамическими указателями траектории движения, Задние датчики парковки, Передние датчики парковки, Круговой обзор • Светодиодные фары • Система доступа в салон без ключа и кнопка запуска двигателя • Премиум-аудиосистема KRELL: 12 динамиков, вкл. сабвуфер, внешний усилитель • Интеграция со смартфонами (Apple CarPlay™/Android Auto™) • Вентиляция и подогрев передних сидений • Раздельные сиденья 2-го ряда (компоновка 2:2:3), вентиляция и подогрев сидений 2-го ряда • Подогрев сидений 3-го ряда • Датчик дождя и Датчик света • Автоматическое переключение ближний/дальний свет (HBA) • Электропривод двери багажника с системой автоматического открывания • Самозатемняющееся внутрисалонное зеркало • Система кругового обзора (SVM) • Система обзора слепых зон (BVM) • Цифровая приборная панель с диагональю 12,3” • Проекция показаний приборов на лобовое стекло • Электропривод подъема/складывания сидений третьего ряда • Память положения водительского сиденья, рулевого колеса, наружных зеркал заднего вида, положения показаний проекционного дисплея для двух водителей • Складывание спинки второго ряда сидений одним нажатием из багажника • Интеллектуальный круиз-контроль с функцией полной остановки и начала движения • Трехзонный климат-контроль • Остекление с дополнительной шумоизоляцией (лобовое и передние боковые стёкла) • Отделка потолка и стоек замшей • Отделка сидений кожей Nappa • Фонари заднего хода с проекцией на дорожное покрытие ________________________________________________   «ДАВ-АВТО» - официальный дилер HYUNDAI в Перми и Пермском крае. Находимся по адресу: г.Пермь, ул.Героев Хасана, д.76 ________________________________________________ Так же при покупке нового HYUNDAI в нашем дилерском центре «ДАВ-АВТО» Вы можете: · Получить специальные условия по автокредитованию · Обменять свой автомобиль на новый по программе Trade-In · Получить специальные условия по страхованию автомобиля · Пройти полное сервисное обслуживание Вашего автомобиля ________________________________________________ *Стоимость автомобиля указана с учётом специальных условий. *Автомобиль без пробега по РФ, не ставился на учёт в России.  Стоимость автомобиля с учетом скидок от дилера 5 900 000р. Скидка по программе Трейд-Ин 150 000 р Скидка по программе автокредитования 150 000 р Максимальная скидка 300 000 р. Стоимость автомобиля без учета скидок 6 200 000 р</t>
+          <t>✔️ 1 Владелец✔️ 2 Комплекта ключей✔️ Полный привод✔️ Классическая автоматическая коробка переключения передач✔️ Экономичный атмосферный двигатель✔️Выгода при обмене 90 000 рублей;✔️Выгода при оформление в кредит 130 000 рублей.📲 Мы можем отправить Вам ссылку на бесплатный отчет Autoteka. Для этого напишите в сообщение:" Ваш мобильный телефон - autoteka" Спектр услуг МОТОР ЛЕНД:🟣 Трейд-ин — обмен Вашего автомобиля на новый или с пробегом;🟣 Срочный выкуп Вашего автомобиля. Деньги в день обращения — в течение 30 минут;🟣 Выкуп кредитных автомобилей. Погашение кредита за Вас;🟣 Кредитование, более 20 банков партнёров;🟣 Доступен кредит без первоначального взноса по 2 документам;🟣 Страхование КАСКО, ОСАГО.📌 Мы находимся по адресу: г. Санкт-Петербург, пр-т Ириновский 10, Официальный дилер КИА МОТОР ЛЕНД.👍 Работаем ежедневно с 09:00 до 20:00.☎ Звоните нам, а лучше приезжайте уже сегодня. Мы всегда рады видеть Вас!</t>
         </is>
       </c>
       <c r="AD11" t="inlineStr">
         <is>
-          <t>Базовая</t>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AE11" t="inlineStr">
+        <is>
+          <t>55000 км</t>
+        </is>
+      </c>
+      <c r="AF11" t="inlineStr">
+        <is>
+          <t>Comfort, Luxe, Prestige, Luxe+, UEFA Europa League, Edition Plus, Prestige Black Edition</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Hyundai Elantra, 2022</t>
+          <t>Skoda Rapid, 2016</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Hyundai</t>
+          <t>Skoda</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Elantra</t>
+          <t>Rapid</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>сегодня в 14:16</t>
+          <t>сегодня в 18:04</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2 990 000</t>
+          <t>810 000</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Пермский край, Пермь, ул. Героев Хасана, 76</t>
+          <t>Санкт-Петербург, Московский район</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>https://www.avito.ru/perm/avtomobili/hyundai_elantra_2022_2902655285</t>
+          <t>https://www.avito.ru/sankt-peterburg/avtomobili/skoda_rapid_2016_3087385892</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2016</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>VII (2020—2023)</t>
+          <t>I (2012—2017)</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -2098,12 +2208,12 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>1.6 AT (128 л.с.)</t>
+          <t>1.4 TSI DSG (125 л.с.)</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>1.6 л</t>
+          <t>1.4 л</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
@@ -2113,7 +2223,7 @@
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>Автомат</t>
+          <t>Робот</t>
         </is>
       </c>
       <c r="O12" t="inlineStr">
@@ -2123,12 +2233,12 @@
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>Седан</t>
+          <t>Лифтбек</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>Красный</t>
+          <t>Серебряный</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
@@ -2138,104 +2248,114 @@
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>47 л</t>
+          <t>55 л</t>
         </is>
       </c>
       <c r="T12" t="inlineStr">
         <is>
-          <t>6,9 л/100 км</t>
+          <t>5,3 л/100 км</t>
         </is>
       </c>
       <c r="U12" t="inlineStr">
         <is>
-          <t>11,3 с</t>
+          <t>9 с</t>
         </is>
       </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>4650 мм</t>
+          <t>4483 мм</t>
         </is>
       </c>
       <c r="W12" t="inlineStr">
         <is>
-          <t>1430 мм</t>
+          <t>1461 мм</t>
         </is>
       </c>
       <c r="X12" t="inlineStr">
         <is>
-          <t>150 мм</t>
+          <t>170 мм</t>
         </is>
       </c>
       <c r="Y12" t="inlineStr">
         <is>
-          <t>1585 мм</t>
+          <t>1457 мм</t>
         </is>
       </c>
       <c r="Z12" t="inlineStr">
         <is>
-          <t>1596 мм</t>
+          <t>1494 мм</t>
         </is>
       </c>
       <c r="AA12" t="inlineStr">
         <is>
-          <t>KMHL*************</t>
+          <t>XW8A*************</t>
         </is>
       </c>
       <c r="AB12" t="inlineStr">
         <is>
-          <t>Электронный</t>
-        </is>
-      </c>
-      <c r="AC12" t="inlineStr">
-        <is>
-          <t>На автомобиль действует скидка 10% от указанной стоимости по Г.О.С. программе. ________________________________________________  Особенности комплектации:  • Беспроводное зарядное устройство (стандарт Qi) • Легкосплавные диски 17" с шинами 225/45R17 • Камера заднего вида с динамическими указателями траектории движения, Задние датчики парковки, Передние датчики парковки • Светодиодные фары • Система доступа в салон без ключа и кнопка запуска двигателя • Премиальная аудиосистема Bose (8 динамиков включая сабвуфер) • Интеграция со смартфонами (Apple CarPlay™/Android Auto™) • Вентиляция передних сидений • Подогрев задних сидений • Датчик дождя и Датчик света • Автоматическое переключение ближний/дальний свет (HBA) • Крыша с люком • Электрорегулировки сиденья водителя + поясничная поддержка водителя • Самозатемняющееся внутрисалонное зеркало • Электрорегулировки сиденья переднего пассажира • Система обзора слепых зон (BVM) • Цифровая приборная панель 10,25" • Навигационная система с HD экраном 10,25" (Apple CarPlay™/Android Auto™1) • Комбинация натуральной и искусственной кожи в отделке сидений • Память настроек сиденья водителя (для двух водителей: сиденье, внешние зеркала) • Уникальный цвет салона: Светло-серый Меланж • Интеллектуальный круиз-контроль с функцией полной остановки и начала движения ________________________________________________   «ДАВ-АВТО» - официальный дилер HYUNDAI в Перми и Пермском крае. Находимся по адресу: г.Пермь, ул.Героев Хасана, д.76 ________________________________________________ Так же при покупке нового HYUNDAI в нашем дилерском центре «ДАВ-АВТО» Вы можете: · Получить специальные условия по автокредитованию · Обменять свой автомобиль на новый по программе Trade-In · Получить специальные условия по страхованию автомобиля · Пройти полное сервисное обслуживание Вашего автомобиля ________________________________________________ *Стоимость автомобиля указана с учётом специальных условий. *Автомобиль без пробега по РФ, не ставился на учёт в России.</t>
+          <t>Оригинал</t>
+        </is>
+      </c>
+      <c r="AD12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AE12" t="inlineStr">
+        <is>
+          <t>121980 км</t>
+        </is>
+      </c>
+      <c r="AF12" t="inlineStr">
+        <is>
+          <t>Ambition, Hockey Edition, Monte Carlo, Style, Базовая</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Hyundai Accent, 2023</t>
+          <t>Suzuki SX4, 2008</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Hyundai</t>
+          <t>Suzuki</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Accent</t>
+          <t>SX4</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>сегодня в 14:16</t>
+          <t>сегодня в 17:45</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>от 1 964 600</t>
+          <t>579 000</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Пермский край, Пермь, ул. Спешилова, 105А</t>
+          <t>Санкт-Петербург, пр-т Маршала Жукова, 51</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>https://www.avito.ru/perm/avtomobili/hyundai_accent_2023_3003793017</t>
+          <t>https://www.avito.ru/sankt-peterburg/avtomobili/suzuki_sx4_2008_3150386387</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>2008</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>V рестайлинг (2020—2023)</t>
+          <t>I (2006—2009)</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
@@ -2245,7 +2365,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>1.6 AT (123 л.с.)</t>
+          <t>1.6 MT (106 л.с.)</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -2260,7 +2380,7 @@
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>Автомат</t>
+          <t>Механика</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
@@ -2270,12 +2390,12 @@
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Седан</t>
+          <t>Хетчбек 5-дверный</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>Серый</t>
+          <t>Чёрный</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
@@ -2285,55 +2405,65 @@
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>50 л</t>
+          <t>0 л</t>
         </is>
       </c>
       <c r="T13" t="inlineStr">
         <is>
-          <t>6,6 л/100 км</t>
+          <t>6,8 л/100 км</t>
         </is>
       </c>
       <c r="U13" t="inlineStr">
         <is>
-          <t>11,2 с</t>
+          <t>11 с</t>
         </is>
       </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>4405 мм</t>
+          <t>4100 мм</t>
         </is>
       </c>
       <c r="W13" t="inlineStr">
         <is>
-          <t>1469 мм</t>
+          <t>1565 мм</t>
         </is>
       </c>
       <c r="X13" t="inlineStr">
         <is>
-          <t>160 мм</t>
+          <t>175 мм</t>
         </is>
       </c>
       <c r="Y13" t="inlineStr">
         <is>
-          <t>1516 мм</t>
+          <t>1500 мм</t>
         </is>
       </c>
       <c r="Z13" t="inlineStr">
         <is>
-          <t>1524 мм</t>
+          <t>1495 мм</t>
         </is>
       </c>
       <c r="AA13" t="inlineStr">
         <is>
-          <t>MXHK*************</t>
+          <t>JSAG*************</t>
         </is>
       </c>
       <c r="AC13" t="inlineStr">
         <is>
-          <t>🔥Hyundai Accent - идеальный автомобиль для тех, кому нужен надежный и бюджетный автомобиль без ущерба для комфорта. Этот автомобиль предлагает уникальное сочетание доступности и удобства.🔥 Одной из ключевых особенностей Hyundai Accent является его надежность. Hyundai известен тем, что производит высококачественные и долговечные автомобили, и Accent не является исключением. При регулярном техническом обслуживании этот автомобиль прослужит вам долгие годы без каких-либо серьезных проблем. Несмотря на низкую цену, Accent предлагает множество функций, которые вы ожидаете найти в более дорогом автомобиле, включая комфортабельный салон и передовые функции безопасности. Одним словом, Hyundai Accent - это идеальный автомобиль для тех, кто хочет иметь надежный и бюджетный автомобиль без ущерба для комфорта и стиля. Благодаря своим передовым функциям, топливной экономичности и просторному салону, этот автомобиль обязательно удовлетворит потребности любого водителя. Так зачем ждать? Ждём вас в гости за новым Другом! ✅ Автомобиль в наличии на складе в Перми (возможна доставка в любой город присутствия наших автосалонов) ✅ Стоимость автомобиля указана с учетом скидок по программам Trade-In и кредитования ✅ Мы предоставляем несколько вариантов Гарантии на автомобиль ✅ При необходимости, можем предоставить возможность установки любого дополнительного оборудования. ✅ В наших салонах возможен любой тип оплаты: -Наличные / Оплата по счету -Перевод с Юр. Лица (с НДС / без НДС) -Кредит на выгодных условиях (Льготная ставка и оформление без КАСКО) -Лизинг (с НДС / без НДС) 🔥Заказ любого АВТОМОБИЛЯ на ваш выбор ✅ Мы Гарантируем полную Юридическую чистоту сделки и всё оформлением документов берем на себя. ✅ Возможен онлайн просмотр, дополнительные фото и видео материалы. Пишите нам, а лучше звоните! -Подушки безопасности водителя и переднего пассажира -Электронная система курсовой устойчивости ESC -Система предупреждения водителей сзади при экстренном торможении ESS -Система удержания при старте на подъем HAC -Система мониторинга давления в шинах TPMS -Антиблокировочная система тормозов ABS -Центральный замок + Сигнализация + Иммобилайзер -Система вызова экстренных служб -Тканевая обивка сидений -Складывающая спинка заднего сиденья в пропорции 60:40 -Аудиосистема с дисплеем 5“ (Radio + RDS) + Bluetooth -USB порт для зарядки внешних устройств -Карман для хранения вещей в спинке сиденья переднего пассажира -Подогрев передних сидений -Кондиционер -Электрорегулировка и подогрев зеркал заднего вида -Ручная регулировка сиденья водителя по высоте -Ручная регулировка рулевого колеса по высоте -Датчик наружней температуры -Стальные диски 15“ с шинами 185/65R15 -Дневные ходовые огни -Окрашенные ручки дверей и бампера в цвет кузова -Передние брызговики -Неполноразмерное запасное колесо</t>
+          <t>Код автомобиля: Ю-42. Автомобиль принят по программе Trade In. Проведена комплексная техническая диагностика. Комплектация: - кондиционер - электропривод и подогрев зеркал - электростеклоподъемники - противотуманные фары - аудиосистема - стальные диски - иммобилайзер Возможна продажа в кредит. Возможен обмен на Ваш автомобиль. ДЦ «Аларм-Моторс Юго-Запад». Проспект Маршала Жукова д.51.</t>
         </is>
       </c>
       <c r="AD13" t="inlineStr">
+        <is>
+          <t>4+</t>
+        </is>
+      </c>
+      <c r="AE13" t="inlineStr">
+        <is>
+          <t>201000 км</t>
+        </is>
+      </c>
+      <c r="AF13" t="inlineStr">
         <is>
           <t>Базовая</t>
         </is>
@@ -2342,47 +2472,47 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Hyundai Elantra, 2022</t>
+          <t>Land Rover Freelander, 2008</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Hyundai</t>
+          <t>Land</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Elantra</t>
+          <t>Rover</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>сегодня в 14:16</t>
+          <t>вчера в 18:06</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2 990 000</t>
+          <t>799 000</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Пермский край, Пермь, ул. Героев Хасана, 76</t>
+          <t>Санкт-Петербург, Пискарёвский пр-т, 25</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>https://www.avito.ru/perm/avtomobili/hyundai_elantra_2022_2902655285</t>
+          <t>https://www.avito.ru/sankt-peterburg/avtomobili/land_rover_freelander_2008_3130273101</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2008</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>VII (2020—2023)</t>
+          <t>II (2006—2010)</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
@@ -2392,12 +2522,12 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>1.6 AT (128 л.с.)</t>
+          <t>3.2 AT (233 л.с.)</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>1.6 л</t>
+          <t>3.2 л</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
@@ -2412,17 +2542,17 @@
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Передний</t>
+          <t>Полный</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Седан</t>
+          <t>Внедорожник 5-дверный</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>Красный</t>
+          <t>Синий</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
@@ -2432,104 +2562,104 @@
       </c>
       <c r="S14" t="inlineStr">
         <is>
-          <t>47 л</t>
+          <t>70 л</t>
         </is>
       </c>
       <c r="T14" t="inlineStr">
         <is>
-          <t>6,9 л/100 км</t>
+          <t>10,7 л/100 км</t>
         </is>
       </c>
       <c r="U14" t="inlineStr">
         <is>
-          <t>11,3 с</t>
+          <t>8,9 с</t>
         </is>
       </c>
       <c r="V14" t="inlineStr">
         <is>
-          <t>4650 мм</t>
+          <t>4500 мм</t>
         </is>
       </c>
       <c r="W14" t="inlineStr">
         <is>
-          <t>1430 мм</t>
+          <t>1740 мм</t>
         </is>
       </c>
       <c r="X14" t="inlineStr">
         <is>
-          <t>150 мм</t>
-        </is>
-      </c>
-      <c r="Y14" t="inlineStr">
-        <is>
-          <t>1585 мм</t>
-        </is>
-      </c>
-      <c r="Z14" t="inlineStr">
-        <is>
-          <t>1596 мм</t>
+          <t>210 мм</t>
         </is>
       </c>
       <c r="AA14" t="inlineStr">
         <is>
-          <t>KMHL*************</t>
+          <t>SALF*************</t>
         </is>
       </c>
       <c r="AB14" t="inlineStr">
         <is>
-          <t>Электронный</t>
-        </is>
-      </c>
-      <c r="AC14" t="inlineStr">
-        <is>
-          <t>На автомобиль действует скидка 10% от указанной стоимости по Г.О.С. программе. ________________________________________________  Особенности комплектации:  • Беспроводное зарядное устройство (стандарт Qi) • Легкосплавные диски 17" с шинами 225/45R17 • Камера заднего вида с динамическими указателями траектории движения, Задние датчики парковки, Передние датчики парковки • Светодиодные фары • Система доступа в салон без ключа и кнопка запуска двигателя • Премиальная аудиосистема Bose (8 динамиков включая сабвуфер) • Интеграция со смартфонами (Apple CarPlay™/Android Auto™) • Вентиляция передних сидений • Подогрев задних сидений • Датчик дождя и Датчик света • Автоматическое переключение ближний/дальний свет (HBA) • Крыша с люком • Электрорегулировки сиденья водителя + поясничная поддержка водителя • Самозатемняющееся внутрисалонное зеркало • Электрорегулировки сиденья переднего пассажира • Система обзора слепых зон (BVM) • Цифровая приборная панель 10,25" • Навигационная система с HD экраном 10,25" (Apple CarPlay™/Android Auto™1) • Комбинация натуральной и искусственной кожи в отделке сидений • Память настроек сиденья водителя (для двух водителей: сиденье, внешние зеркала) • Уникальный цвет салона: Светло-серый Меланж • Интеллектуальный круиз-контроль с функцией полной остановки и начала движения ________________________________________________   «ДАВ-АВТО» - официальный дилер HYUNDAI в Перми и Пермском крае. Находимся по адресу: г.Пермь, ул.Героев Хасана, д.76 ________________________________________________ Так же при покупке нового HYUNDAI в нашем дилерском центре «ДАВ-АВТО» Вы можете: · Получить специальные условия по автокредитованию · Обменять свой автомобиль на новый по программе Trade-In · Получить специальные условия по страхованию автомобиля · Пройти полное сервисное обслуживание Вашего автомобиля ________________________________________________ *Стоимость автомобиля указана с учётом специальных условий. *Автомобиль без пробега по РФ, не ставился на учёт в России.</t>
+          <t>Дубликат</t>
+        </is>
+      </c>
+      <c r="AD14" t="inlineStr">
+        <is>
+          <t>4+</t>
+        </is>
+      </c>
+      <c r="AE14" t="inlineStr">
+        <is>
+          <t>220000 км</t>
+        </is>
+      </c>
+      <c r="AF14" t="inlineStr">
+        <is>
+          <t>HSE, SE</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Hyundai Accent, 2023</t>
+          <t>Toyota Corolla, 2007</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Hyundai</t>
+          <t>Toyota</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Accent</t>
+          <t>Corolla</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>сегодня в 14:16</t>
+          <t>сегодня в 17:48</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>от 1 964 600</t>
+          <t>569 000</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Пермский край, Пермь, ул. Спешилова, 105А</t>
+          <t>Санкт-Петербург, Выборгское ш., 27к2Б</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>https://www.avito.ru/perm/avtomobili/hyundai_accent_2023_3003793017</t>
+          <t>https://www.avito.ru/sankt-peterburg/avtomobili/toyota_corolla_2007_3068641572</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>2007</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>V рестайлинг (2020—2023)</t>
+          <t>X (2006—2013)</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -2539,7 +2669,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>1.6 AT (123 л.с.)</t>
+          <t>1.6 AMT (124 л.с.)</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
@@ -2554,7 +2684,7 @@
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>Автомат</t>
+          <t>Робот</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
@@ -2569,7 +2699,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>Серый</t>
+          <t>Серебряный</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
@@ -2579,200 +2709,1147 @@
       </c>
       <c r="S15" t="inlineStr">
         <is>
-          <t>50 л</t>
+          <t>55 л</t>
         </is>
       </c>
       <c r="T15" t="inlineStr">
         <is>
-          <t>6,6 л/100 км</t>
+          <t>6,7 л/100 км</t>
         </is>
       </c>
       <c r="U15" t="inlineStr">
         <is>
-          <t>11,2 с</t>
+          <t>12,1 с</t>
         </is>
       </c>
       <c r="V15" t="inlineStr">
         <is>
-          <t>4405 мм</t>
+          <t>4540 мм</t>
         </is>
       </c>
       <c r="W15" t="inlineStr">
         <is>
-          <t>1469 мм</t>
+          <t>1470 мм</t>
         </is>
       </c>
       <c r="X15" t="inlineStr">
         <is>
-          <t>160 мм</t>
+          <t>150 мм</t>
         </is>
       </c>
       <c r="Y15" t="inlineStr">
         <is>
-          <t>1516 мм</t>
+          <t>1525 мм</t>
         </is>
       </c>
       <c r="Z15" t="inlineStr">
         <is>
-          <t>1524 мм</t>
+          <t>1520 мм</t>
         </is>
       </c>
       <c r="AA15" t="inlineStr">
         <is>
-          <t>MXHK*************</t>
+          <t>JTNB*************</t>
         </is>
       </c>
       <c r="AC15" t="inlineStr">
         <is>
-          <t>🔥Hyundai Accent - идеальный автомобиль для тех, кому нужен надежный и бюджетный автомобиль без ущерба для комфорта. Этот автомобиль предлагает уникальное сочетание доступности и удобства.🔥 Одной из ключевых особенностей Hyundai Accent является его надежность. Hyundai известен тем, что производит высококачественные и долговечные автомобили, и Accent не является исключением. При регулярном техническом обслуживании этот автомобиль прослужит вам долгие годы без каких-либо серьезных проблем. Несмотря на низкую цену, Accent предлагает множество функций, которые вы ожидаете найти в более дорогом автомобиле, включая комфортабельный салон и передовые функции безопасности. Одним словом, Hyundai Accent - это идеальный автомобиль для тех, кто хочет иметь надежный и бюджетный автомобиль без ущерба для комфорта и стиля. Благодаря своим передовым функциям, топливной экономичности и просторному салону, этот автомобиль обязательно удовлетворит потребности любого водителя. Так зачем ждать? Ждём вас в гости за новым Другом! ✅ Автомобиль в наличии на складе в Перми (возможна доставка в любой город присутствия наших автосалонов) ✅ Стоимость автомобиля указана с учетом скидок по программам Trade-In и кредитования ✅ Мы предоставляем несколько вариантов Гарантии на автомобиль ✅ При необходимости, можем предоставить возможность установки любого дополнительного оборудования. ✅ В наших салонах возможен любой тип оплаты: -Наличные / Оплата по счету -Перевод с Юр. Лица (с НДС / без НДС) -Кредит на выгодных условиях (Льготная ставка и оформление без КАСКО) -Лизинг (с НДС / без НДС) 🔥Заказ любого АВТОМОБИЛЯ на ваш выбор ✅ Мы Гарантируем полную Юридическую чистоту сделки и всё оформлением документов берем на себя. ✅ Возможен онлайн просмотр, дополнительные фото и видео материалы. Пишите нам, а лучше звоните! -Подушки безопасности водителя и переднего пассажира -Электронная система курсовой устойчивости ESC -Система предупреждения водителей сзади при экстренном торможении ESS -Система удержания при старте на подъем HAC -Система мониторинга давления в шинах TPMS -Антиблокировочная система тормозов ABS -Центральный замок + Сигнализация + Иммобилайзер -Система вызова экстренных служб -Тканевая обивка сидений -Складывающая спинка заднего сиденья в пропорции 60:40 -Аудиосистема с дисплеем 5“ (Radio + RDS) + Bluetooth -USB порт для зарядки внешних устройств -Карман для хранения вещей в спинке сиденья переднего пассажира -Подогрев передних сидений -Кондиционер -Электрорегулировка и подогрев зеркал заднего вида -Ручная регулировка сиденья водителя по высоте -Ручная регулировка рулевого колеса по высоте -Датчик наружней температуры -Стальные диски 15“ с шинами 185/65R15 -Дневные ходовые огни -Окрашенные ручки дверей и бампера в цвет кузова -Передние брызговики -Неполноразмерное запасное колесо</t>
+          <t>Купить автомобиль с пробегом у официального дилера «Форсаж» Volkswagen, УАЗ, HAVAL— это безопасно, быстро и комфортно.⭐ЧЕСТНАЯ ЦЕНА - цена без скрытых условий, за наличный расчет⭐⭐ Хорошая комплектация⭐ установлена магнитола андроид с камерой заднего вида⭐установлена кнопка старт/стоп⭐ Установлена сигнализация с автозапуском⭐ Проведена комплексная диагностика⭐ Полный комплект документов✅Честная процентная ставка по кредиту от 9,5% годовых ✅Кредиты с временной регистрацией✅Кредит ПЛАТИ МЕНЬШЕ: кредит с остаточным платежом✅Кредит без первоначального взноса!✅ Кредитование от 12 месяцев до 96 месяцев (8 лет)✅Уровень одобрений 95%✅Покупка авто одним днём Для кредита:❕Нужен только паспорт❕ ✔95% одобрений✔🔹Сотрудничаем с 1️⃣7️⃣ надежными банками🔹🚘Форсаж🚘 Почему именно мы?📍Выгодные условия приобретения📍Предпродажная подготовка📍Гарантия юридической чистоты. Наши эксперты проводят сверку номерных агрегатов📍Предоставление полного пакета документов для регистрации автомобиля в органах ГИБДД📍Проверенные автомобили с пробегом, прошедшие полную комплексную техническую диагностику📍Специальные предложения на сервисное обслуживание и дополнительное оборудование📍Уникальное предложение по кредиту от банков-партнеров📍Примем ваш авто в зачет с выгодой до 30 000р📞Пишите и звоните прямо сейчас! Рады видеть Вас каждый день с 9 до 21 по адресу: Выборгское шоссе, 27 к2БМесто осмотраОсмотреть автомобиль можно по адресу: Санкт-Петербург, Выборгское шоссе 27, Volkswagen Форсаж ОзеркиХарактеристикиРоботизированная коробка передач, 5 ст.Комплектация «Элеганс»:Активная безопасность:Антиблокировочная системаСистема курсовой устойчивостиПассивная безопасность:Подушки безопасности водителяПодушки безопасности пассажираБоковые передние подушки безопасностиПротивоугонная система:Сигнализация с обратной связьюДистанционный запуск двигателяИммобилайзерЦентральный замокПомощь при вождении:Бортовой компьютерКруиз-контрольКамера заднего видаКомфорт:Гидро усилитель руляРегулировка руляРегулировка сиденья пассажира в двух плоскостяхЭлектростеклоподъемники передние и задниеЭлектропривод зеркалУправление климатом и обогрев:КондиционерКлимат-контроль 1-зонныйПодогрев сидений водителя и пассажираОбогрев зеркалОбогрев заднего стеклаМультимедиа и навигация:CDDVDUSBРадиоTVBluetoothAUXРозетка 12VСалон и интерьер:Тканевая обивка салонаСветлый салонКожаный рульСкладывающееся заднее сидениеЭкстерьер:Литые легкосплавные дискиЗадние тонированные стеклаОсвещение:Противотуманные фарыОгни дневного ходаКорректор фар с ручным управлениемКомплектность:Отметки ТО ЧастичноСервисная книжка2 комплекта ключейКомплект ковриков</t>
         </is>
       </c>
       <c r="AD15" t="inlineStr">
         <is>
-          <t>Базовая</t>
+          <t>4+</t>
+        </is>
+      </c>
+      <c r="AE15" t="inlineStr">
+        <is>
+          <t>251211 км</t>
+        </is>
+      </c>
+      <c r="AF15" t="inlineStr">
+        <is>
+          <t>Базовая, Elegance, Prestige</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Subaru Forester, 2022</t>
+          <t>Kia Rio, 2017</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
+          <t>Kia</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Rio</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>сегодня в 18:04</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>999 000</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург, Московский район</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>https://www.avito.ru/sankt-peterburg/avtomobili/kia_rio_2017_3087367154</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>2017</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>IV (2017—2020)</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Не битый</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>1.6 AT (123 л.с.)</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>1.6 л</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>Бензин</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>Автомат</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>Передний</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>Седан</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>Синий</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>Левый</t>
+        </is>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>0 л</t>
+        </is>
+      </c>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>6,6 л/100 км</t>
+        </is>
+      </c>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>11,2 с</t>
+        </is>
+      </c>
+      <c r="V16" t="inlineStr">
+        <is>
+          <t>4400 мм</t>
+        </is>
+      </c>
+      <c r="W16" t="inlineStr">
+        <is>
+          <t>1470 мм</t>
+        </is>
+      </c>
+      <c r="X16" t="inlineStr">
+        <is>
+          <t>160 мм</t>
+        </is>
+      </c>
+      <c r="AA16" t="inlineStr">
+        <is>
+          <t>Z94C*************</t>
+        </is>
+      </c>
+      <c r="AB16" t="inlineStr">
+        <is>
+          <t>Оригинал</t>
+        </is>
+      </c>
+      <c r="AD16" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AE16" t="inlineStr">
+        <is>
+          <t>108270 км</t>
+        </is>
+      </c>
+      <c r="AF16" t="inlineStr">
+        <is>
+          <t>Comfort, Edition Plus, Luxe, Luxe 2018 FWC, Premium, Prestige, Luxe RED Line</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Mercedes-Benz GLK-класс, 2014</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Mercedes-Benz</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>GLK-класс</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>сегодня в 12:13</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>1 599 000</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург, пр-т Маршала Жукова, 78</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>https://www.avito.ru/sankt-peterburg/avtomobili/mercedes-benz_glk-klass_2014_3064668740</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>X204 рестайлинг (2012—2015)</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Не битый</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>GLK 220d 2.1 4MATIC 7G-Tronic (170 л.с.)</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>2.1 л</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>Дизель</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>Автомат</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>Полный</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>Внедорожник 5-дверный</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>Белый</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>Левый</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>59 л</t>
+        </is>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>6,1 л/100 км</t>
+        </is>
+      </c>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>8,8 с</t>
+        </is>
+      </c>
+      <c r="V17" t="inlineStr">
+        <is>
+          <t>4536 мм</t>
+        </is>
+      </c>
+      <c r="W17" t="inlineStr">
+        <is>
+          <t>1669 мм</t>
+        </is>
+      </c>
+      <c r="X17" t="inlineStr">
+        <is>
+          <t>187 мм</t>
+        </is>
+      </c>
+      <c r="AA17" t="inlineStr">
+        <is>
+          <t>WDC2*************</t>
+        </is>
+      </c>
+      <c r="AC17" t="inlineStr">
+        <is>
+          <t>А также, воспользовавшись нашей программой Trade-in, получите помимо выгодной цены за ваш старый автомобиль - скидку до 100 000 рублей.  Все автомобили, представленные в продаже проходят диагностику . Так же была осуществлена полная предпродажная подготовка и полировка кузова.  Предоставляем гарантию юридической чистоты, а так же год технической гарантии на двигатель и КПП в письменной форме.  Каждому нашему клиенту мы дарим на выбор: Комплект новой резины, Полное комплексное ТО, Страховой полис ОСАГО сроком на 3 месяца.  Действует программа льготного автокредитования со ставкой по кредиту от 4,9%!  Помимо покупки за наличные или обмена по Trade-In, вы можете воспользоваться одной из нескольких выгодных программ автокредитования от наших банков-партнеров. Минимальный пакет документов, быстрое решение, низкая процентная ставка. "CARVANA" - один из лидеров по продажам автомобилей с пробегом в Санкт-Петербурге!  Преимущества автокредитования:  •Кредитная ставка от 4,9% годовых; •Взнос от 0%; •Документы: паспорт и водительское удостоверение; •Около 30 программ кредитования; •Лимит кредитования от 50 000 до 2 500 000 рублей; •Без оформления КАСКО; •Срок кредитования от 6 месяцев до 7 лет; •Возможность досрочного погашения без комиссий и штрафов  Приглашаем на бесплатный тест-драйв! Более подробную информацию можно получить по указанному номеру телефона.  Более подробную информацию по наличию автомобилей Вы можете узнать на нашем официальном сайте. Для этого откройте карточку магазина, которая находится под номером телефона, далее переходите в раздел "контакты" и переходите по ссылке.</t>
+        </is>
+      </c>
+      <c r="AD17" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AE17" t="inlineStr">
+        <is>
+          <t>144166 км</t>
+        </is>
+      </c>
+      <c r="AF17" t="inlineStr">
+        <is>
+          <t>Blueefficiency, Blueefficiency Особая серия, Особая серия</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Ford Mondeo, 2014</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Ford</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Mondeo</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>сегодня в 17:45</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>999 000</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург, пр-т Маршала Жукова, 51</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>https://www.avito.ru/sankt-peterburg/avtomobili/ford_mondeo_2014_3150634979</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>IV рестайлинг (2010—2014)</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Не битый</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>2.0 TDCi AT (140 л.с.)</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>2.0 л</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>Дизель</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>Автомат</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>Передний</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>Седан</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>Коричневый</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>Левый</t>
+        </is>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>70 л</t>
+        </is>
+      </c>
+      <c r="T18" t="inlineStr">
+        <is>
+          <t>7,1 л/100 км</t>
+        </is>
+      </c>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>10,2 с</t>
+        </is>
+      </c>
+      <c r="V18" t="inlineStr">
+        <is>
+          <t>4784 мм</t>
+        </is>
+      </c>
+      <c r="W18" t="inlineStr">
+        <is>
+          <t>1500 мм</t>
+        </is>
+      </c>
+      <c r="X18" t="inlineStr">
+        <is>
+          <t>130 мм</t>
+        </is>
+      </c>
+      <c r="Y18" t="inlineStr">
+        <is>
+          <t>1588 мм</t>
+        </is>
+      </c>
+      <c r="Z18" t="inlineStr">
+        <is>
+          <t>1605 мм</t>
+        </is>
+      </c>
+      <c r="AA18" t="inlineStr">
+        <is>
+          <t>X9FD*************</t>
+        </is>
+      </c>
+      <c r="AC18" t="inlineStr">
+        <is>
+          <t>Код автомобиля: Ю-101. Автомобиль принят по программе Trade In. Проведена комплексная техническая диагностика. ПТС оригинал. Два владельца. Комплектация Titanium: - тканевый салон - климат-контроль - электропривод и подогрев зеркал - ABS/ESP - AUX/USB/Bluetooth - противотуманные фары - подогрев передних сидений - аудиосистема с управлением на руле - круиз-контроль - датчики дождя/света - легкосплавные диски - ксенон - омыватель фар - датчики парковки передние и задние - иммобилайзер - крепление для детского кресла (isofix/latch) Возможна продажа в кредит. Возможен обмен на Ваш автомобиль. ДЦ «Аларм-Моторс Юго-Запад». Проспект Маршала Жукова д.51.</t>
+        </is>
+      </c>
+      <c r="AD18" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AE18" t="inlineStr">
+        <is>
+          <t>191000 км</t>
+        </is>
+      </c>
+      <c r="AF18" t="inlineStr">
+        <is>
+          <t>Titanium, Titanium Black, Базовая</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Hyundai Palisade, 2020</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Hyundai</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Palisade</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>сегодня в 12:00</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>3 899 000</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург, пр-т Маршала Жукова, 78</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>https://www.avito.ru/sankt-peterburg/avtomobili/hyundai_palisade_2020_3160578362</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>I (2018—2022)</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Не битый</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>2.2 CRDi 4WD AT (200 л.с.)</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>2.2 л</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>Дизель</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>Автомат</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>Полный</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>Внедорожник 5-дверный</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>Чёрный</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>Левый</t>
+        </is>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>71 л</t>
+        </is>
+      </c>
+      <c r="T19" t="inlineStr">
+        <is>
+          <t>7,3 л/100 км</t>
+        </is>
+      </c>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>10,5 с</t>
+        </is>
+      </c>
+      <c r="V19" t="inlineStr">
+        <is>
+          <t>4980 мм</t>
+        </is>
+      </c>
+      <c r="W19" t="inlineStr">
+        <is>
+          <t>1750 мм</t>
+        </is>
+      </c>
+      <c r="X19" t="inlineStr">
+        <is>
+          <t>203 мм</t>
+        </is>
+      </c>
+      <c r="Y19" t="inlineStr">
+        <is>
+          <t>1708 мм</t>
+        </is>
+      </c>
+      <c r="Z19" t="inlineStr">
+        <is>
+          <t>1716 мм</t>
+        </is>
+      </c>
+      <c r="AA19" t="inlineStr">
+        <is>
+          <t>KMHR*************</t>
+        </is>
+      </c>
+      <c r="AC19" t="inlineStr">
+        <is>
+          <t>Получите дополнительную скидку до 300 000 рублей при покупке данного автомобиля в кредит!  А также, воспользовавшись нашей программой Trade-in, получите помимо выгодной цены за ваш старый автомобиль - скидку до 100 000 рублей.  Все автомобили, представленные в продаже проходят диагностику . Так же была осуществлена полная предпродажная подготовка и полировка кузова.  Предоставляем гарантию юридической чистоты, а так же год технической гарантии на двигатель и КПП в письменной форме.  Каждому нашему клиенту мы дарим на выбор: Комплект новой резины, Полное комплексное ТО, Страховой полис ОСАГО сроком на 3 месяца.  Действует программа льготного автокредитования со ставкой по кредиту от 4,9%!  Помимо покупки за наличные или обмена по Trade-In, вы можете воспользоваться одной из нескольких выгодных программ автокредитования от наших банков-партнеров. Минимальный пакет документов, быстрое решение, низкая процентная ставка. "CARVANA" - один из лидеров по продажам автомобилей с пробегом в Санкт-Петербурге!  Преимущества автокредитования:  •Кредитная ставка от 4,9% годовых; •Взнос от 0%; •Документы: паспорт и водительское удостоверение; •Около 30 программ кредитования; •Лимит кредитования от 50 000 до 2 500 000 рублей; •Без оформления КАСКО; •Срок кредитования от 6 месяцев до 7 лет; •Возможность досрочного погашения без комиссий и штрафов  Приглашаем на бесплатный тест-драйв! Более подробную информацию можно получить по указанному номеру телефона.  Более подробную информацию по наличию автомобилей Вы можете узнать на нашем официальном сайте. Для этого откройте карточку магазина, которая находится под номером телефона, далее переходите в раздел "контакты" и переходите по ссылке.</t>
+        </is>
+      </c>
+      <c r="AD19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AE19" t="inlineStr">
+        <is>
+          <t>55330 км</t>
+        </is>
+      </c>
+      <c r="AF19" t="inlineStr">
+        <is>
+          <t>Prestige, High-Tech, Lifestyle, Lifestyle + Smart Sense, Prestige + Smart Sense, Специальная серия «Cosmos» (7 мест), Специальная серия «Cosmos» (8 мест), High-Tech + Nappa</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Subaru Forester, 2012</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
           <t>Subaru</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C20" t="inlineStr">
         <is>
           <t>Forester</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>сегодня в 14:14</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>от 5 075 700</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>Пермский край, Пермь, Подлесная ул., 47А</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>https://www.avito.ru/perm/avtomobili/subaru_forester_2022_2521673519</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>SK рестайлинг (2021—2023)</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>сегодня в 17:48</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>1 099 000</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург, Выборгское ш., 27к2Б</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>https://www.avito.ru/sankt-peterburg/avtomobili/subaru_forester_2012_3100583956</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>2012</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>SH рестайлинг (2010—2013)</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
         <is>
           <t>Не битый</t>
         </is>
       </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>2.5 4WD CVT (185 л.с.)</t>
-        </is>
-      </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>2.5 л</t>
-        </is>
-      </c>
-      <c r="M16" t="inlineStr">
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>2.0 4WD MT (150 л.с.)</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>2.0 л</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
         <is>
           <t>Бензин</t>
         </is>
       </c>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>Вариатор</t>
-        </is>
-      </c>
-      <c r="O16" t="inlineStr">
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>Механика</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
         <is>
           <t>Полный</t>
         </is>
       </c>
-      <c r="P16" t="inlineStr">
+      <c r="P20" t="inlineStr">
         <is>
           <t>Внедорожник 5-дверный</t>
         </is>
       </c>
-      <c r="Q16" t="inlineStr">
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>Серебряный</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>Левый</t>
+        </is>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>60 л</t>
+        </is>
+      </c>
+      <c r="T20" t="inlineStr">
+        <is>
+          <t>8,1 л/100 км</t>
+        </is>
+      </c>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>10,7 с</t>
+        </is>
+      </c>
+      <c r="V20" t="inlineStr">
+        <is>
+          <t>4560 мм</t>
+        </is>
+      </c>
+      <c r="W20" t="inlineStr">
+        <is>
+          <t>1700 мм</t>
+        </is>
+      </c>
+      <c r="X20" t="inlineStr">
+        <is>
+          <t>215 мм</t>
+        </is>
+      </c>
+      <c r="Y20" t="inlineStr">
+        <is>
+          <t>1530 мм</t>
+        </is>
+      </c>
+      <c r="Z20" t="inlineStr">
+        <is>
+          <t>1530 мм</t>
+        </is>
+      </c>
+      <c r="AA20" t="inlineStr">
+        <is>
+          <t>JF1S*************</t>
+        </is>
+      </c>
+      <c r="AC20" t="inlineStr">
+        <is>
+          <t>Купить автомобиль с пробегом у официального дилера «Форсаж» Volkswagen, УАЗ, HAVAL— это безопасно, быстро и комфортно.⭐ЧЕСТНАЯ ЦЕНА - цена без скрытых условий, за наличный расчет⭐ Оригинал ПТС⭐ один собственник по птс⭐ Родной пробег⭐ Проведена комплексная диагностика⭐ Полный комплект ключей и документов✅Честная процентная ставка по кредиту от 9,5% годовых ✅Кредиты с временной регистрацией✅Кредит ПЛАТИ МЕНЬШЕ: кредит с остаточным платежом✅Кредит без первоначального взноса!✅ Кредитование от 12 месяцев до 96 месяцев (8 лет)✅Уровень одобрений 95%✅Покупка авто одним днём Для кредита:❕Нужен только паспорт❕ ✔95% одобрений✔🔹Сотрудничаем с 1️⃣7️⃣ надежными банками🔹🚘Форсаж🚘 Почему именно мы?📍Выгодные условия приобретения📍Предпродажная подготовка📍Гарантия юридической чистоты. Наши эксперты проводят сверку номерных агрегатов📍Предоставление полного пакета документов для регистрации автомобиля в органах ГИБДД📍Проверенные автомобили с пробегом, прошедшие полную комплексную техническую диагностику📍Специальные предложения на сервисное обслуживание и дополнительное оборудование📍Уникальное предложение по кредиту от банков-партнеров📍Примем ваш авто в зачет с выгодой до 30 000р📞Пишите и звоните прямо сейчас! Рады видеть Вас каждый день с 9 до 21 по адресу: Выборгское шоссе, 27 к2БПТС оригинал.Место осмотраОсмотреть автомобиль можно по адресу: Санкт-Петербург, Выборгское шоссе 27, Volkswagen Форсаж ОзеркиКомплектация «YV»:Активная безопасность:Антиблокировочная системаСистема курсовой устойчивостиПассивная безопасность:Подушки безопасности водителяПодушки безопасности пассажираБоковые передние подушки безопасностиОконные шторки безопасностиСистема крепления детских автокреселПротивоугонная система:СигнализацияИммобилайзерЦентральный замокПомощь при вождении:Бортовой компьютерКруиз-контрольКамера заднего видаСистема помощи при старте в горуКомфорт:Усилитель руляРегулировка руляЭлектростеклоподъемники передние и задниеЭлектропривод зеркалУправление климатом и обогрев:КондиционерКлимат-контроль 1-зонныйПодогрев сидений водителя и пассажираОбогрев зеркалОбогрев зоны стеклоочистителейМультимедиа и навигация:CDBluetoothAUXМультифункциональное рулевое колесоСалон и интерьер:Тканевая обивка салонаКожаный рульСкладывающееся заднее сидениеТретий задний подголовникОсвещение:Противотуманные фарыОмыватель фарКомплектность:2 комплекта ключей</t>
+        </is>
+      </c>
+      <c r="AD20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AE20" t="inlineStr">
+        <is>
+          <t>205943 км</t>
+        </is>
+      </c>
+      <c r="AF20" t="inlineStr">
+        <is>
+          <t>2M, TV, WV, YV</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Volkswagen Polo, 2019</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Volkswagen</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Polo</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>сегодня в 18:03</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>985 000</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург, 2 линия</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>https://www.avito.ru/sankt-peterburg/avtomobili/volkswagen_polo_2019_3087435150</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>V рестайлинг (2015—2020)</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Не битый</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>1.6 MPI AT (110 л.с.)</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>1.6 л</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>Бензин</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>Автомат</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>Передний</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>Седан</t>
+        </is>
+      </c>
+      <c r="Q21" t="inlineStr">
         <is>
           <t>Синий</t>
         </is>
       </c>
-      <c r="R16" t="inlineStr">
+      <c r="R21" t="inlineStr">
         <is>
           <t>Левый</t>
         </is>
       </c>
-      <c r="S16" t="inlineStr">
-        <is>
-          <t>63 л</t>
-        </is>
-      </c>
-      <c r="T16" t="inlineStr">
-        <is>
-          <t>7,4 л/100 км</t>
-        </is>
-      </c>
-      <c r="U16" t="inlineStr">
-        <is>
-          <t>9,5 с</t>
-        </is>
-      </c>
-      <c r="V16" t="inlineStr">
-        <is>
-          <t>4640 мм</t>
-        </is>
-      </c>
-      <c r="W16" t="inlineStr">
-        <is>
-          <t>1730 мм</t>
-        </is>
-      </c>
-      <c r="X16" t="inlineStr">
-        <is>
-          <t>220 мм</t>
-        </is>
-      </c>
-      <c r="Y16" t="inlineStr">
-        <is>
-          <t>1565 мм</t>
-        </is>
-      </c>
-      <c r="Z16" t="inlineStr">
-        <is>
-          <t>1570 мм</t>
-        </is>
-      </c>
-      <c r="AA16" t="inlineStr">
-        <is>
-          <t>JF1S*************</t>
-        </is>
-      </c>
-      <c r="AB16" t="inlineStr"/>
-      <c r="AC16" t="inlineStr">
-        <is>
-          <t>Автомобиль SUBARU «FORESTER» MY22 в комплектации SPORT 2.5L в наличии!Стоимость автомобиля указана с полным НДС. Автомобиль дилерский, НЕ параллельный импорт.В данную комплектацию входит:- Система управления температурой в салоне жестами;- Подрулевые лепестки переключения передач;- Мультимедиа-система с дисплеем 8,0", и 6 динамиками;- Регулировка наклона спинок задних сидений;- Камера переднего и бокового обзора;- Система динамического освещения поворотов (SRH);- Система автоматического управления дальним светом (HBA);- Система X-mode (помощь по бездорожью, 2 режима);- Пакет Sport (экстерьер/интерьер);- и многое другое...Данный автомобиль уже ждет Вас в салоне по адресу: г. Пермь, ул. Подлесная 47А.</t>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>55 л</t>
+        </is>
+      </c>
+      <c r="T21" t="inlineStr">
+        <is>
+          <t>5,9 л/100 км</t>
+        </is>
+      </c>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>11,7 с</t>
+        </is>
+      </c>
+      <c r="V21" t="inlineStr">
+        <is>
+          <t>4390 мм</t>
+        </is>
+      </c>
+      <c r="W21" t="inlineStr">
+        <is>
+          <t>1467 мм</t>
+        </is>
+      </c>
+      <c r="X21" t="inlineStr">
+        <is>
+          <t>163 мм</t>
+        </is>
+      </c>
+      <c r="Y21" t="inlineStr">
+        <is>
+          <t>1457 мм</t>
+        </is>
+      </c>
+      <c r="Z21" t="inlineStr">
+        <is>
+          <t>1500 мм</t>
+        </is>
+      </c>
+      <c r="AA21" t="inlineStr">
+        <is>
+          <t>XW8Z*************</t>
+        </is>
+      </c>
+      <c r="AB21" t="inlineStr">
+        <is>
+          <t>Оригинал</t>
+        </is>
+      </c>
+      <c r="AD21" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AE21" t="inlineStr">
+        <is>
+          <t>77480 км</t>
+        </is>
+      </c>
+      <c r="AF21" t="inlineStr">
+        <is>
+          <t>Comfortline, Drive, Highline, Joy, Trendline, Allstar, Life, Connect, Football Edition, Select</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>BMW 5 серия, 2019</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>BMW</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>сегодня в 12:01</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>3 890 000</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург, ул. Тельмана, 29</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>https://www.avito.ru/sankt-peterburg/avtomobili/bmw_5_seriya_2019_3165146451</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>G30/G31 (2016—2020)</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Не битый</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>520d 2.0 xDrive Steptronic (190 л.с.)</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>2.0 л</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>Дизель</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>Автомат</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>Полный</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>Седан</t>
+        </is>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>Белый</t>
+        </is>
+      </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>Левый</t>
+        </is>
+      </c>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>66 л</t>
+        </is>
+      </c>
+      <c r="T22" t="inlineStr">
+        <is>
+          <t>4,8 л/100 км</t>
+        </is>
+      </c>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>7,6 с</t>
+        </is>
+      </c>
+      <c r="V22" t="inlineStr">
+        <is>
+          <t>4962 мм</t>
+        </is>
+      </c>
+      <c r="W22" t="inlineStr">
+        <is>
+          <t>1479 мм</t>
+        </is>
+      </c>
+      <c r="X22" t="inlineStr">
+        <is>
+          <t>144 мм</t>
+        </is>
+      </c>
+      <c r="Y22" t="inlineStr">
+        <is>
+          <t>1605 мм</t>
+        </is>
+      </c>
+      <c r="Z22" t="inlineStr">
+        <is>
+          <t>1630 мм</t>
+        </is>
+      </c>
+      <c r="AA22" t="inlineStr">
+        <is>
+          <t>WBAJ*************</t>
+        </is>
+      </c>
+      <c r="AB22" t="inlineStr"/>
+      <c r="AC22" t="inlineStr">
+        <is>
+          <t>Представляем Вашему вниманию BMW 520d xDrive! Полный привод!✅ M-Sport.✅ 1 Владелец.✅ Без ДТП.✅ Оригинальный пробег.✅ Отличное внешнее и техническое состояние.✅ Обслуживание на официальном дилере в Германии.✅ Автомобиль поставлен на учет на Дилерский Центр. Автомобиль представлен официальным дилером "Аксель-Сити Невский"  Более 250 проверенных автомобилей с пробегом в наличии.	Проверка автомобиля по 300 пунктам перед продажей экспертами нашего сервисного центра.	Возможность приобретения в кредит и лизинг.	Программа трейд-ин и выкуп авто (экспресс оценка и выдача денег за несколько часов).	Гарантия юридической чистоты сделки.	Страховые продукты любого уровня сложности по лучшей стоимости.	Мы готовы предоставить дополнительную гарантию на автомобиль.Аксель-Сити Невский В СЛУЧАЕ ОБНАРУЖЕНИЯ СКРЫТЫХ ДЕФЕКТОВ – ВОЗВРАТ ДЕНЕЖНЫХ СРЕДСТВ В ТЕЧЕНИЕ 14 ДНЕЙ С МОМЕНТА ПОКУПКИКомфортная зона ожидания и уютное кафе с ароматным кофе и свежей выпечкой.Будем рады Вас видеть в нашем дилерском центре по адресу: ул. Тельмана, д. 29. Время работы с 09:00 до 21:00 ежедневно.ПТС оригинал.Место осмотраОсмотреть автомобиль можно по адресу: Санкт-Петербург, ул. Тельмана, д. 29Комплектация «520d xDrive»:Активная безопасность:Антиблокировочная системаАнтипробуксовочная системаСистема курсовой устойчивостиСистема помощи при экстренном торможенииДатчик давления в шинахЭРА-ГЛОНАССПассивная безопасность:Подушки безопасности водителяПодушки безопасности пассажираБоковые передние подушки безопасностиОконные шторки безопасностиСистема крепления детских автокреселПротивоугонная система:ИммобилайзерЦентральный замокПомощь при вождении:Бортовой компьютерКруиз-контрольПарктроник передний и заднийСистема помощи при старте в горуДатчик светаДатчик дождяКомфорт:Активный усилитель руляЗапуск двигателя с кнопкиСистема “старт-стоп”Регулировка руляЭлектростеклоподъемники передние и задниеЭлектропривод зеркалДекоративное освещение салонаУправление климатом и обогрев:Климат-контроль 2-зонныйПодогрев сидений водителя и пассажираПодогрев руляОбогрев зеркалОбогрев форсунок стеклоомывателейМультимедиа и навигация:CDUSBBluetoothAUXМультифункциональное рулевое колесоСалон и интерьер:Велюровая обивка салонаАлькантаровая обивка салонаКомбинированная обивка салонаТемный салонКожаный рульТретий задний подголовникПередний центральный подлокотникПрикуриватель и пепельницаЭкстерьер:Размер дисков 17″Освещение:Светодиодные фарыПротивотуманные фарыОгни дневного ходаКорректор фарКомплектность:2 комплекта ключей</t>
+        </is>
+      </c>
+      <c r="AD22" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AE22" t="inlineStr">
+        <is>
+          <t>53300 км</t>
+        </is>
+      </c>
+      <c r="AF22" t="inlineStr">
+        <is>
+          <t>Base, Business, Exclusive, M Sport</t>
         </is>
       </c>
     </row>

</xml_diff>